<commit_message>
fix data,remove unnecessary screenshot
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="11" activeTab="13" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPR06_LoanMerge" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -118,7 +118,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -146,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -331,6 +337,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,7 +1402,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -1532,7 +1539,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -1669,7 +1676,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -1801,7 +1808,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -1926,7 +1933,7 @@
     <row r="6">
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -1938,7 +1945,7 @@
     <row r="7">
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -1950,7 +1957,7 @@
     <row r="8">
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
@@ -1962,7 +1969,7 @@
     <row r="9">
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
@@ -1974,7 +1981,7 @@
     <row r="10">
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E10" s="47" t="n"/>
@@ -1987,7 +1994,7 @@
     <row r="11">
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E11" s="47" t="n"/>
@@ -2000,7 +2007,7 @@
     <row r="12">
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E12" s="47" t="n"/>
@@ -2219,7 +2226,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="26" t="inlineStr">
@@ -2354,7 +2361,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="26" t="inlineStr">
@@ -2485,7 +2492,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="26" t="inlineStr">
@@ -2624,7 +2631,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="26" t="inlineStr">
@@ -2755,7 +2762,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D6" s="26" t="inlineStr">
@@ -2894,7 +2901,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D7" s="26" t="inlineStr">
@@ -3090,7 +3097,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="28" t="inlineStr">
@@ -3544,8 +3551,8 @@
   </sheetPr>
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3781,7 +3788,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -3968,7 +3975,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -4395,7 +4402,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="8" t="inlineStr">
@@ -4781,7 +4788,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -4960,7 +4967,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -5139,7 +5146,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -5314,7 +5321,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -5876,7 +5883,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="66" t="inlineStr">
@@ -7086,8 +7093,8 @@
   </sheetPr>
   <dimension ref="A1:DY2"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -7126,7 +7133,8 @@
     <col width="43" customWidth="1" style="3" min="32" max="33"/>
     <col width="40.5703125" customWidth="1" style="3" min="34" max="34"/>
     <col width="41.28515625" customWidth="1" style="3" min="35" max="36"/>
-    <col width="14.28515625" customWidth="1" style="3" min="37" max="38"/>
+    <col width="18.7109375" customWidth="1" style="3" min="37" max="37"/>
+    <col width="14.28515625" customWidth="1" style="3" min="38" max="38"/>
     <col width="12.5703125" customWidth="1" style="3" min="39" max="39"/>
     <col width="16.28515625" customWidth="1" style="3" min="40" max="40"/>
     <col width="12.85546875" customWidth="1" style="3" min="41" max="41"/>
@@ -7179,6 +7187,9 @@
     <col width="19" customWidth="1" style="3" min="108" max="108"/>
     <col width="19.28515625" customWidth="1" style="3" min="109" max="109"/>
     <col width="19.140625" customWidth="1" style="3" min="110" max="110"/>
+    <col width="18.85546875" customWidth="1" min="111" max="111"/>
+    <col width="17.7109375" customWidth="1" min="112" max="112"/>
+    <col width="19" customWidth="1" min="113" max="113"/>
     <col width="25.140625" customWidth="1" style="3" min="114" max="114"/>
     <col width="25.85546875" customWidth="1" style="3" min="115" max="115"/>
     <col width="22.42578125" customWidth="1" style="3" min="116" max="116"/>
@@ -7865,10 +7876,8 @@
           <t>Search by Customer ID</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
+      <c r="E2" s="3" t="n">
+        <v>1213044</v>
       </c>
       <c r="F2" s="16" t="inlineStr">
         <is>
@@ -7915,10 +7924,8 @@
           <t>Work Fax</t>
         </is>
       </c>
-      <c r="O2" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
+      <c r="O2" s="3" t="n">
+        <v>1213044</v>
       </c>
       <c r="P2" s="17" t="inlineStr">
         <is>
@@ -8461,8 +8468,8 @@
   </sheetPr>
   <dimension ref="A1:CI3"/>
   <sheetViews>
-    <sheetView topLeftCell="CA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9011,12 +9018,12 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>UAT118112019165520</t>
+          <t>UAT126082020152139</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -9034,10 +9041,8 @@
           <t>Sales Group 1</t>
         </is>
       </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
+      <c r="J2" s="3" t="n">
+        <v>1213044</v>
       </c>
       <c r="K2" s="3" t="inlineStr">
         <is>
@@ -9076,7 +9081,7 @@
       </c>
       <c r="R2" s="3" t="inlineStr">
         <is>
-          <t>%DBU</t>
+          <t>%OBU</t>
         </is>
       </c>
       <c r="S2" s="3" t="inlineStr">
@@ -9294,7 +9299,7 @@
       <c r="BL2" s="26" t="n"/>
       <c r="BM2" s="26" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTH BANK AU-OBU</t>
         </is>
       </c>
       <c r="BN2" s="26" t="inlineStr">
@@ -9309,7 +9314,7 @@
       </c>
       <c r="BP2" s="26" t="inlineStr">
         <is>
-          <t>RTGS</t>
+          <t>IMT</t>
         </is>
       </c>
       <c r="BQ2" s="26" t="inlineStr">
@@ -9359,7 +9364,7 @@
       </c>
       <c r="BZ2" s="26" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTH BANK AU-OBU</t>
         </is>
       </c>
       <c r="CA2" s="26" t="inlineStr">
@@ -9495,10 +9500,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9524,18 +9529,18 @@
     <col width="33.28515625" customWidth="1" style="3" min="19" max="19"/>
     <col width="19.42578125" customWidth="1" style="3" min="20" max="20"/>
     <col width="32.7109375" customWidth="1" style="3" min="21" max="21"/>
-    <col width="21" customWidth="1" style="3" min="22" max="22"/>
-    <col width="18.28515625" customWidth="1" style="3" min="23" max="23"/>
-    <col width="20" customWidth="1" style="3" min="24" max="24"/>
-    <col width="19.85546875" customWidth="1" style="3" min="25" max="26"/>
-    <col width="25.85546875" customWidth="1" style="3" min="27" max="28"/>
-    <col width="26.5703125" customWidth="1" style="3" min="29" max="30"/>
-    <col width="25.5703125" customWidth="1" style="3" min="31" max="32"/>
-    <col width="26.85546875" customWidth="1" style="3" min="33" max="34"/>
-    <col width="14.85546875" customWidth="1" style="3" min="35" max="36"/>
-    <col width="20.42578125" customWidth="1" style="3" min="37" max="38"/>
-    <col width="33" customWidth="1" style="3" min="39" max="40"/>
-    <col width="16.85546875" customWidth="1" style="3" min="41" max="42"/>
+    <col width="21" customWidth="1" style="3" min="22" max="23"/>
+    <col width="18.28515625" customWidth="1" style="3" min="24" max="24"/>
+    <col width="20" customWidth="1" style="3" min="25" max="25"/>
+    <col width="19.85546875" customWidth="1" style="3" min="26" max="27"/>
+    <col width="25.85546875" customWidth="1" style="3" min="28" max="29"/>
+    <col width="26.5703125" customWidth="1" style="3" min="30" max="31"/>
+    <col width="25.5703125" customWidth="1" style="3" min="32" max="33"/>
+    <col width="26.85546875" customWidth="1" style="3" min="34" max="35"/>
+    <col width="14.85546875" customWidth="1" style="3" min="36" max="37"/>
+    <col width="20.42578125" customWidth="1" style="3" min="38" max="39"/>
+    <col width="33" customWidth="1" style="3" min="40" max="41"/>
+    <col width="16.85546875" customWidth="1" style="3" min="42" max="43"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="29" thickBot="1">
@@ -9649,102 +9654,107 @@
           <t>Facility_SGLocation</t>
         </is>
       </c>
-      <c r="W1" s="29" t="inlineStr">
+      <c r="W1" s="70" t="inlineStr">
+        <is>
+          <t>Facility_Borrower</t>
+        </is>
+      </c>
+      <c r="X1" s="29" t="inlineStr">
         <is>
           <t>Facility_Borrower1</t>
         </is>
       </c>
-      <c r="X1" s="29" t="inlineStr">
+      <c r="Y1" s="29" t="inlineStr">
         <is>
           <t>Facility_Borrower2</t>
         </is>
       </c>
-      <c r="Y1" s="29" t="inlineStr">
+      <c r="Z1" s="29" t="inlineStr">
         <is>
           <t>Borrower_Currency1</t>
         </is>
       </c>
-      <c r="Z1" s="29" t="inlineStr">
+      <c r="AA1" s="29" t="inlineStr">
         <is>
           <t>Borrower_Currency2</t>
         </is>
       </c>
-      <c r="AA1" s="29" t="inlineStr">
+      <c r="AB1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerMaturity1</t>
         </is>
       </c>
-      <c r="AB1" s="29" t="inlineStr">
+      <c r="AC1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerMaturity2</t>
         </is>
       </c>
-      <c r="AC1" s="29" t="inlineStr">
+      <c r="AD1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerSGName1</t>
         </is>
       </c>
-      <c r="AD1" s="29" t="inlineStr">
+      <c r="AE1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerSGName2</t>
         </is>
       </c>
-      <c r="AE1" s="29" t="inlineStr">
+      <c r="AF1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerPercent1</t>
         </is>
       </c>
-      <c r="AF1" s="29" t="inlineStr">
+      <c r="AG1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerPercent2</t>
         </is>
       </c>
-      <c r="AG1" s="29" t="inlineStr">
+      <c r="AH1" s="29" t="inlineStr">
         <is>
           <t>SublimitCust_EffectiveDate1</t>
         </is>
       </c>
-      <c r="AH1" s="29" t="inlineStr">
+      <c r="AI1" s="29" t="inlineStr">
         <is>
           <t>SublimitCust_EffectiveDate2</t>
         </is>
       </c>
-      <c r="AI1" s="29" t="inlineStr">
+      <c r="AJ1" s="29" t="inlineStr">
         <is>
           <t>CurrencyLimit1</t>
         </is>
       </c>
-      <c r="AJ1" s="29" t="inlineStr">
+      <c r="AK1" s="29" t="inlineStr">
         <is>
           <t>CurrencyLimit2</t>
         </is>
       </c>
-      <c r="AK1" s="29" t="inlineStr">
+      <c r="AL1" s="29" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit1</t>
         </is>
       </c>
-      <c r="AL1" s="29" t="inlineStr">
+      <c r="AM1" s="29" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit2</t>
         </is>
       </c>
-      <c r="AM1" s="29" t="inlineStr">
+      <c r="AN1" s="29" t="inlineStr">
         <is>
           <t>Facility_CustomerServicingGroup1</t>
         </is>
       </c>
-      <c r="AN1" s="29" t="inlineStr">
+      <c r="AO1" s="29" t="inlineStr">
         <is>
           <t>Facility_CustomerServicingGroup2</t>
         </is>
       </c>
-      <c r="AO1" s="29" t="inlineStr">
+      <c r="AP1" s="29" t="inlineStr">
         <is>
           <t>Facility_SGAlias1</t>
         </is>
       </c>
-      <c r="AP1" s="29" t="inlineStr">
+      <c r="AQ1" s="29" t="inlineStr">
         <is>
           <t>Facility_SGAlias2</t>
         </is>
@@ -9768,7 +9778,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -9861,142 +9871,145 @@
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="W2" s="3" t="inlineStr">
+      <c r="W2" t="n">
+        <v>1213044</v>
+      </c>
+      <c r="X2" s="26" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="X2" s="3" t="inlineStr">
+      <c r="Y2" s="26" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="Y2" s="26" t="inlineStr">
+      <c r="Z2" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="Z2" s="26" t="inlineStr">
+      <c r="AA2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AA2" s="26" t="inlineStr">
+      <c r="AB2" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AB2" s="26" t="inlineStr">
+      <c r="AC2" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AC2" s="26" t="inlineStr">
+      <c r="AD2" s="26" t="inlineStr">
         <is>
           <t>WICK</t>
         </is>
       </c>
-      <c r="AD2" s="26" t="inlineStr">
+      <c r="AE2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AE2" s="26" t="inlineStr">
+      <c r="AF2" s="26" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="AF2" s="26" t="inlineStr">
+      <c r="AG2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AG2" s="26" t="inlineStr">
+      <c r="AH2" s="26" t="inlineStr">
         <is>
           <t>15-Dec-2017</t>
         </is>
       </c>
-      <c r="AH2" s="26" t="inlineStr">
+      <c r="AI2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AI2" s="26" t="inlineStr">
+      <c r="AJ2" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AJ2" s="26" t="inlineStr">
+      <c r="AK2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AK2" s="26" t="inlineStr">
+      <c r="AL2" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AL2" s="26" t="inlineStr">
+      <c r="AM2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AM2" s="26" t="inlineStr">
+      <c r="AN2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AN2" s="26" t="inlineStr">
+      <c r="AO2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AO2" s="26" t="inlineStr">
+      <c r="AP2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AP2" s="26" t="inlineStr">
+      <c r="AQ2" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AQ2" s="3" t="inlineStr">
+      <c r="AR2" s="3" t="inlineStr">
         <is>
           <t>1213218</t>
         </is>
       </c>
-      <c r="AR2" s="3" t="inlineStr">
+      <c r="AS2" s="3" t="inlineStr">
         <is>
           <t>1213218</t>
         </is>
       </c>
-      <c r="AS2" s="3" t="inlineStr">
+      <c r="AT2" s="3" t="inlineStr">
         <is>
           <t>1411409</t>
         </is>
       </c>
-      <c r="AT2" s="3" t="inlineStr">
+      <c r="AU2" s="3" t="inlineStr">
         <is>
           <t>1114300</t>
         </is>
       </c>
-      <c r="AU2" s="3" t="inlineStr">
+      <c r="AV2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AV2" s="3" t="inlineStr">
+      <c r="AW2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AW2" s="3" t="inlineStr">
+      <c r="AX2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AX2" s="3" t="inlineStr">
+      <c r="AY2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
@@ -10020,7 +10033,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -10113,137 +10126,140 @@
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="W3" s="3" t="inlineStr">
+      <c r="W3" t="n">
+        <v>1213044</v>
+      </c>
+      <c r="X3" s="26" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="X3" s="3" t="inlineStr">
+      <c r="Y3" s="26" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="Y3" s="26" t="inlineStr">
+      <c r="Z3" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="Z3" s="26" t="inlineStr">
+      <c r="AA3" s="26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AA3" s="26" t="inlineStr">
+      <c r="AB3" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AB3" s="26" t="inlineStr">
+      <c r="AC3" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AC3" s="26" t="inlineStr">
+      <c r="AD3" s="26" t="inlineStr">
         <is>
           <t>WICK</t>
         </is>
       </c>
-      <c r="AD3" s="26" t="inlineStr">
+      <c r="AE3" s="26" t="inlineStr">
         <is>
           <t>WICK</t>
         </is>
       </c>
-      <c r="AE3" s="26" t="inlineStr">
+      <c r="AF3" s="26" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="AF3" s="26" t="inlineStr">
+      <c r="AG3" s="26" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="AG3" s="26" t="inlineStr">
+      <c r="AH3" s="26" t="inlineStr">
         <is>
           <t>01-Dec-2017</t>
         </is>
       </c>
-      <c r="AH3" s="26" t="inlineStr">
+      <c r="AI3" s="26" t="inlineStr">
         <is>
           <t>15-Dec-2017</t>
         </is>
       </c>
-      <c r="AI3" s="26" t="inlineStr">
+      <c r="AJ3" s="26" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AJ3" s="26" t="inlineStr">
+      <c r="AK3" s="26" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="AK3" s="26" t="inlineStr">
+      <c r="AL3" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AL3" s="26" t="inlineStr">
+      <c r="AM3" s="26" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="AM3" s="26" t="inlineStr">
+      <c r="AN3" s="26" t="inlineStr">
         <is>
           <t>Commonwealth Bank Australia - DBU</t>
         </is>
       </c>
-      <c r="AN3" s="26" t="inlineStr">
+      <c r="AO3" s="26" t="inlineStr">
         <is>
           <t>Commonwealth Bank Australia - DBU</t>
         </is>
       </c>
-      <c r="AO3" s="26" t="inlineStr">
+      <c r="AP3" s="26" t="inlineStr">
         <is>
           <t>OL</t>
         </is>
       </c>
-      <c r="AP3" s="26" t="inlineStr">
+      <c r="AQ3" s="26" t="inlineStr">
         <is>
           <t>OL</t>
         </is>
       </c>
-      <c r="AQ3" s="3" t="inlineStr">
+      <c r="AR3" s="3" t="inlineStr">
         <is>
           <t>1213218</t>
         </is>
       </c>
-      <c r="AR3" s="3" t="inlineStr">
+      <c r="AS3" s="3" t="inlineStr">
         <is>
           <t>1213218</t>
         </is>
       </c>
-      <c r="AS3" s="3" t="inlineStr">
+      <c r="AT3" s="3" t="inlineStr">
         <is>
           <t>1411409</t>
         </is>
       </c>
-      <c r="AU3" s="3" t="inlineStr">
+      <c r="AV3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AV3" s="3" t="inlineStr">
+      <c r="AW3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AW3" s="3" t="inlineStr">
+      <c r="AX3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AX3" s="3" t="inlineStr">
+      <c r="AY3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
@@ -11991,7 +12007,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -12104,7 +12120,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -12217,7 +12233,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -12321,7 +12337,7 @@
       <c r="A5" s="40" t="n"/>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -12339,7 +12355,7 @@
       <c r="A6" s="40" t="n"/>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -12357,7 +12373,7 @@
       <c r="A7" s="40" t="n"/>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6745 Fixes for EVG_CBAUAT01.robot, 03DealBorrower.robot, GenericKeywords.robot and EVG_CBAUAT01.xlsx.
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="11" activeTab="13" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7860" yWindow="4575" windowWidth="24105" windowHeight="15555" tabRatio="600" firstSheet="5" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPR06_LoanMerge" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -643,8 +643,8 @@
   <dimension ref="A1:CP2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd1213041</t>
+          <t>Sanseera Electronics Ltd 1614804</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="K2" s="8" t="inlineStr">
         <is>
-          <t>Bank,�Domestic Public Company</t>
+          <t>Other Unincorporated Association, Unincorporated Association</t>
         </is>
       </c>
       <c r="L2" s="7" t="inlineStr">
@@ -1207,8 +1207,8 @@
   </sheetPr>
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -1980,7 +1980,7 @@
       <c r="E10" s="47" t="n"/>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
       <c r="E11" s="47" t="n"/>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
       <c r="E12" s="47" t="n"/>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
     </row>
@@ -3544,7 +3544,7 @@
   </sheetPr>
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5491,8 +5491,8 @@
   </sheetPr>
   <dimension ref="A1:HM10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7857,7 +7857,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd1213041</t>
+          <t>Sanseera Electronics Ltd 1614804</t>
         </is>
       </c>
       <c r="D2" s="14" t="inlineStr">
@@ -7867,7 +7867,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1614804</t>
         </is>
       </c>
       <c r="F2" s="16" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6745 Fixes for CBA UAT 01.
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7860" yWindow="4575" windowWidth="24105" windowHeight="15555" tabRatio="600" firstSheet="5" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8430" yWindow="10560" windowWidth="24315" windowHeight="6480" tabRatio="600" firstSheet="10" activeTab="13" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPR06_LoanMerge" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -118,7 +118,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -146,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -331,6 +337,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,8 +650,8 @@
   <dimension ref="A1:CP2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E37" sqref="E37"/>
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1002,7 +1009,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd 1614804</t>
+          <t>Sanseera Electronics Ltd 1913520</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -1017,7 +1024,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -1207,8 +1214,8 @@
   </sheetPr>
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1395,7 +1402,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -1410,7 +1417,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -1532,7 +1539,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -1547,7 +1554,7 @@
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -1669,7 +1676,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -1684,7 +1691,7 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
@@ -1801,7 +1808,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -1816,7 +1823,7 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
@@ -1926,87 +1933,87 @@
     <row r="6">
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E10" s="47" t="n"/>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E11" s="47" t="n"/>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E12" s="47" t="n"/>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
@@ -2219,7 +2226,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="26" t="inlineStr">
@@ -2249,7 +2256,7 @@
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="J2" s="3" t="inlineStr">
@@ -2354,7 +2361,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="26" t="inlineStr">
@@ -2384,7 +2391,7 @@
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
@@ -2485,7 +2492,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="26" t="inlineStr">
@@ -2515,7 +2522,7 @@
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
@@ -2624,7 +2631,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="26" t="inlineStr">
@@ -2654,7 +2661,7 @@
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr">
@@ -2755,7 +2762,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D6" s="26" t="inlineStr">
@@ -2785,7 +2792,7 @@
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="J6" s="3" t="inlineStr">
@@ -2894,7 +2901,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D7" s="26" t="inlineStr">
@@ -2924,7 +2931,7 @@
       </c>
       <c r="I7" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="J7" s="3" t="inlineStr">
@@ -3090,7 +3097,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="28" t="inlineStr">
@@ -3544,8 +3551,8 @@
   </sheetPr>
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3781,7 +3788,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -3901,7 +3908,7 @@
       </c>
       <c r="AA2" s="3" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd1213041</t>
+          <t>Sanseera Electronics Ltd 1913520</t>
         </is>
       </c>
       <c r="AB2" s="26" t="inlineStr">
@@ -3911,7 +3918,7 @@
       </c>
       <c r="AC2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="AD2" s="39" t="inlineStr">
@@ -3968,7 +3975,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -4093,7 +4100,7 @@
       </c>
       <c r="AC3" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="AD3" s="39" t="inlineStr">
@@ -4395,7 +4402,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="8" t="inlineStr">
@@ -4526,7 +4533,7 @@
       </c>
       <c r="AD2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="AE2" s="26" t="inlineStr">
@@ -4781,7 +4788,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -4832,7 +4839,7 @@
       </c>
       <c r="N2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="O2" s="3" t="inlineStr">
@@ -4960,7 +4967,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -5011,7 +5018,7 @@
       </c>
       <c r="N3" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="O3" s="3" t="inlineStr">
@@ -5139,7 +5146,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -5190,7 +5197,7 @@
       </c>
       <c r="N4" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="O4" s="3" t="inlineStr">
@@ -5314,7 +5321,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -5365,7 +5372,7 @@
       </c>
       <c r="N5" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="O5" s="3" t="inlineStr">
@@ -5491,8 +5498,8 @@
   </sheetPr>
   <dimension ref="A1:HM10"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -5876,7 +5883,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="66" t="inlineStr">
@@ -5956,7 +5963,7 @@
       </c>
       <c r="S2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="T2" s="3" t="inlineStr">
@@ -6533,7 +6540,7 @@
       </c>
       <c r="S3" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="T3" s="3" t="inlineStr">
@@ -7020,42 +7027,42 @@
     <row r="4">
       <c r="S4" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="S5" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="S6" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="S7" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="S8" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="S9" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
@@ -7067,7 +7074,7 @@
       </c>
       <c r="S10" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
     </row>
@@ -7086,8 +7093,8 @@
   </sheetPr>
   <dimension ref="A1:DY2"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -7126,7 +7133,8 @@
     <col width="43" customWidth="1" style="3" min="32" max="33"/>
     <col width="40.5703125" customWidth="1" style="3" min="34" max="34"/>
     <col width="41.28515625" customWidth="1" style="3" min="35" max="36"/>
-    <col width="14.28515625" customWidth="1" style="3" min="37" max="38"/>
+    <col width="18.7109375" customWidth="1" style="3" min="37" max="37"/>
+    <col width="14.28515625" customWidth="1" style="3" min="38" max="38"/>
     <col width="12.5703125" customWidth="1" style="3" min="39" max="39"/>
     <col width="16.28515625" customWidth="1" style="3" min="40" max="40"/>
     <col width="12.85546875" customWidth="1" style="3" min="41" max="41"/>
@@ -7179,6 +7187,9 @@
     <col width="19" customWidth="1" style="3" min="108" max="108"/>
     <col width="19.28515625" customWidth="1" style="3" min="109" max="109"/>
     <col width="19.140625" customWidth="1" style="3" min="110" max="110"/>
+    <col width="18.85546875" customWidth="1" min="111" max="111"/>
+    <col width="17.7109375" customWidth="1" min="112" max="112"/>
+    <col width="19" customWidth="1" min="113" max="113"/>
     <col width="25.140625" customWidth="1" style="3" min="114" max="114"/>
     <col width="25.85546875" customWidth="1" style="3" min="115" max="115"/>
     <col width="22.42578125" customWidth="1" style="3" min="116" max="116"/>
@@ -7857,7 +7868,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd 1614804</t>
+          <t>Sanseera Electronics Ltd 1913520</t>
         </is>
       </c>
       <c r="D2" s="14" t="inlineStr">
@@ -7867,7 +7878,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>1614804</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="F2" s="16" t="inlineStr">
@@ -7917,7 +7928,7 @@
       </c>
       <c r="O2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="P2" s="17" t="inlineStr">
@@ -8461,8 +8472,8 @@
   </sheetPr>
   <dimension ref="A1:CI3"/>
   <sheetViews>
-    <sheetView topLeftCell="CA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9011,12 +9022,12 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>UAT118112019165520</t>
+          <t>UAT126082020152139</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -9036,7 +9047,7 @@
       </c>
       <c r="J2" s="3" t="inlineStr">
         <is>
-          <t>1213044</t>
+          <t>1913520</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
@@ -9076,7 +9087,7 @@
       </c>
       <c r="R2" s="3" t="inlineStr">
         <is>
-          <t>%DBU</t>
+          <t>%OBU</t>
         </is>
       </c>
       <c r="S2" s="3" t="inlineStr">
@@ -9294,7 +9305,7 @@
       <c r="BL2" s="26" t="n"/>
       <c r="BM2" s="26" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTH BANK AU-OBU</t>
         </is>
       </c>
       <c r="BN2" s="26" t="inlineStr">
@@ -9309,7 +9320,7 @@
       </c>
       <c r="BP2" s="26" t="inlineStr">
         <is>
-          <t>RTGS</t>
+          <t>IMT</t>
         </is>
       </c>
       <c r="BQ2" s="26" t="inlineStr">
@@ -9359,7 +9370,7 @@
       </c>
       <c r="BZ2" s="26" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTH BANK AU-OBU</t>
         </is>
       </c>
       <c r="CA2" s="26" t="inlineStr">
@@ -9495,10 +9506,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -9524,18 +9535,18 @@
     <col width="33.28515625" customWidth="1" style="3" min="19" max="19"/>
     <col width="19.42578125" customWidth="1" style="3" min="20" max="20"/>
     <col width="32.7109375" customWidth="1" style="3" min="21" max="21"/>
-    <col width="21" customWidth="1" style="3" min="22" max="22"/>
-    <col width="18.28515625" customWidth="1" style="3" min="23" max="23"/>
-    <col width="20" customWidth="1" style="3" min="24" max="24"/>
-    <col width="19.85546875" customWidth="1" style="3" min="25" max="26"/>
-    <col width="25.85546875" customWidth="1" style="3" min="27" max="28"/>
-    <col width="26.5703125" customWidth="1" style="3" min="29" max="30"/>
-    <col width="25.5703125" customWidth="1" style="3" min="31" max="32"/>
-    <col width="26.85546875" customWidth="1" style="3" min="33" max="34"/>
-    <col width="14.85546875" customWidth="1" style="3" min="35" max="36"/>
-    <col width="20.42578125" customWidth="1" style="3" min="37" max="38"/>
-    <col width="33" customWidth="1" style="3" min="39" max="40"/>
-    <col width="16.85546875" customWidth="1" style="3" min="41" max="42"/>
+    <col width="21" customWidth="1" style="3" min="22" max="23"/>
+    <col width="18.28515625" customWidth="1" style="3" min="24" max="24"/>
+    <col width="20" customWidth="1" style="3" min="25" max="25"/>
+    <col width="19.85546875" customWidth="1" style="3" min="26" max="27"/>
+    <col width="25.85546875" customWidth="1" style="3" min="28" max="29"/>
+    <col width="26.5703125" customWidth="1" style="3" min="30" max="31"/>
+    <col width="25.5703125" customWidth="1" style="3" min="32" max="33"/>
+    <col width="26.85546875" customWidth="1" style="3" min="34" max="35"/>
+    <col width="14.85546875" customWidth="1" style="3" min="36" max="37"/>
+    <col width="20.42578125" customWidth="1" style="3" min="38" max="39"/>
+    <col width="33" customWidth="1" style="3" min="40" max="41"/>
+    <col width="16.85546875" customWidth="1" style="3" min="42" max="43"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="29" thickBot="1">
@@ -9649,102 +9660,107 @@
           <t>Facility_SGLocation</t>
         </is>
       </c>
-      <c r="W1" s="29" t="inlineStr">
+      <c r="W1" s="70" t="inlineStr">
+        <is>
+          <t>Facility_Borrower</t>
+        </is>
+      </c>
+      <c r="X1" s="29" t="inlineStr">
         <is>
           <t>Facility_Borrower1</t>
         </is>
       </c>
-      <c r="X1" s="29" t="inlineStr">
+      <c r="Y1" s="29" t="inlineStr">
         <is>
           <t>Facility_Borrower2</t>
         </is>
       </c>
-      <c r="Y1" s="29" t="inlineStr">
+      <c r="Z1" s="29" t="inlineStr">
         <is>
           <t>Borrower_Currency1</t>
         </is>
       </c>
-      <c r="Z1" s="29" t="inlineStr">
+      <c r="AA1" s="29" t="inlineStr">
         <is>
           <t>Borrower_Currency2</t>
         </is>
       </c>
-      <c r="AA1" s="29" t="inlineStr">
+      <c r="AB1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerMaturity1</t>
         </is>
       </c>
-      <c r="AB1" s="29" t="inlineStr">
+      <c r="AC1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerMaturity2</t>
         </is>
       </c>
-      <c r="AC1" s="29" t="inlineStr">
+      <c r="AD1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerSGName1</t>
         </is>
       </c>
-      <c r="AD1" s="29" t="inlineStr">
+      <c r="AE1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerSGName2</t>
         </is>
       </c>
-      <c r="AE1" s="29" t="inlineStr">
+      <c r="AF1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerPercent1</t>
         </is>
       </c>
-      <c r="AF1" s="29" t="inlineStr">
+      <c r="AG1" s="29" t="inlineStr">
         <is>
           <t>Facility_BorrowerPercent2</t>
         </is>
       </c>
-      <c r="AG1" s="29" t="inlineStr">
+      <c r="AH1" s="29" t="inlineStr">
         <is>
           <t>SublimitCust_EffectiveDate1</t>
         </is>
       </c>
-      <c r="AH1" s="29" t="inlineStr">
+      <c r="AI1" s="29" t="inlineStr">
         <is>
           <t>SublimitCust_EffectiveDate2</t>
         </is>
       </c>
-      <c r="AI1" s="29" t="inlineStr">
+      <c r="AJ1" s="29" t="inlineStr">
         <is>
           <t>CurrencyLimit1</t>
         </is>
       </c>
-      <c r="AJ1" s="29" t="inlineStr">
+      <c r="AK1" s="29" t="inlineStr">
         <is>
           <t>CurrencyLimit2</t>
         </is>
       </c>
-      <c r="AK1" s="29" t="inlineStr">
+      <c r="AL1" s="29" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit1</t>
         </is>
       </c>
-      <c r="AL1" s="29" t="inlineStr">
+      <c r="AM1" s="29" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit2</t>
         </is>
       </c>
-      <c r="AM1" s="29" t="inlineStr">
+      <c r="AN1" s="29" t="inlineStr">
         <is>
           <t>Facility_CustomerServicingGroup1</t>
         </is>
       </c>
-      <c r="AN1" s="29" t="inlineStr">
+      <c r="AO1" s="29" t="inlineStr">
         <is>
           <t>Facility_CustomerServicingGroup2</t>
         </is>
       </c>
-      <c r="AO1" s="29" t="inlineStr">
+      <c r="AP1" s="29" t="inlineStr">
         <is>
           <t>Facility_SGAlias1</t>
         </is>
       </c>
-      <c r="AP1" s="29" t="inlineStr">
+      <c r="AQ1" s="29" t="inlineStr">
         <is>
           <t>Facility_SGAlias2</t>
         </is>
@@ -9768,7 +9784,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -9861,142 +9877,145 @@
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="W2" s="3" t="inlineStr">
+      <c r="W2" t="n">
+        <v>1213044</v>
+      </c>
+      <c r="X2" s="26" t="inlineStr">
+        <is>
+          <t>1913520</t>
+        </is>
+      </c>
+      <c r="Y2" s="26" t="inlineStr">
+        <is>
+          <t>1913520</t>
+        </is>
+      </c>
+      <c r="Z2" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AA2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AB2" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AC2" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AD2" s="26" t="inlineStr">
+        <is>
+          <t>WICK</t>
+        </is>
+      </c>
+      <c r="AE2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AF2" s="26" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="AG2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AH2" s="26" t="inlineStr">
+        <is>
+          <t>15-Dec-2017</t>
+        </is>
+      </c>
+      <c r="AI2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AJ2" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AK2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AL2" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AM2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AN2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AO2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AP2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AQ2" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AR2" s="3" t="inlineStr">
+        <is>
+          <t>1213218</t>
+        </is>
+      </c>
+      <c r="AS2" s="3" t="inlineStr">
+        <is>
+          <t>1213218</t>
+        </is>
+      </c>
+      <c r="AT2" s="3" t="inlineStr">
+        <is>
+          <t>1411409</t>
+        </is>
+      </c>
+      <c r="AU2" s="3" t="inlineStr">
+        <is>
+          <t>1114300</t>
+        </is>
+      </c>
+      <c r="AV2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="X2" s="3" t="inlineStr">
+      <c r="AW2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="Y2" s="26" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
-      <c r="Z2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AA2" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AB2" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AC2" s="26" t="inlineStr">
-        <is>
-          <t>WICK</t>
-        </is>
-      </c>
-      <c r="AD2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AE2" s="26" t="inlineStr">
-        <is>
-          <t>100.000000%</t>
-        </is>
-      </c>
-      <c r="AF2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AG2" s="26" t="inlineStr">
-        <is>
-          <t>15-Dec-2017</t>
-        </is>
-      </c>
-      <c r="AH2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AI2" s="26" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
-      <c r="AJ2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AK2" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AL2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AM2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AN2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AO2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AP2" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AQ2" s="3" t="inlineStr">
-        <is>
-          <t>1213218</t>
-        </is>
-      </c>
-      <c r="AR2" s="3" t="inlineStr">
-        <is>
-          <t>1213218</t>
-        </is>
-      </c>
-      <c r="AS2" s="3" t="inlineStr">
-        <is>
-          <t>1411409</t>
-        </is>
-      </c>
-      <c r="AT2" s="3" t="inlineStr">
-        <is>
-          <t>1114300</t>
-        </is>
-      </c>
-      <c r="AU2" s="3" t="inlineStr">
+      <c r="AX2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AV2" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
-      </c>
-      <c r="AW2" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
-      </c>
-      <c r="AX2" s="3" t="inlineStr">
+      <c r="AY2" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
@@ -10020,7 +10039,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -10113,137 +10132,140 @@
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="W3" s="3" t="inlineStr">
+      <c r="W3" t="n">
+        <v>1213044</v>
+      </c>
+      <c r="X3" s="26" t="inlineStr">
+        <is>
+          <t>1913520</t>
+        </is>
+      </c>
+      <c r="Y3" s="26" t="inlineStr">
+        <is>
+          <t>1913520</t>
+        </is>
+      </c>
+      <c r="Z3" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AA3" s="26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AB3" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AC3" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AD3" s="26" t="inlineStr">
+        <is>
+          <t>WICK</t>
+        </is>
+      </c>
+      <c r="AE3" s="26" t="inlineStr">
+        <is>
+          <t>WICK</t>
+        </is>
+      </c>
+      <c r="AF3" s="26" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="AG3" s="26" t="inlineStr">
+        <is>
+          <t>100.000000%</t>
+        </is>
+      </c>
+      <c r="AH3" s="26" t="inlineStr">
+        <is>
+          <t>01-Dec-2017</t>
+        </is>
+      </c>
+      <c r="AI3" s="26" t="inlineStr">
+        <is>
+          <t>15-Dec-2017</t>
+        </is>
+      </c>
+      <c r="AJ3" s="26" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="AK3" s="26" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="AL3" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AM3" s="26" t="inlineStr">
+        <is>
+          <t>FLOAT</t>
+        </is>
+      </c>
+      <c r="AN3" s="26" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank Australia - DBU</t>
+        </is>
+      </c>
+      <c r="AO3" s="26" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank Australia - DBU</t>
+        </is>
+      </c>
+      <c r="AP3" s="26" t="inlineStr">
+        <is>
+          <t>OL</t>
+        </is>
+      </c>
+      <c r="AQ3" s="26" t="inlineStr">
+        <is>
+          <t>OL</t>
+        </is>
+      </c>
+      <c r="AR3" s="3" t="inlineStr">
+        <is>
+          <t>1213218</t>
+        </is>
+      </c>
+      <c r="AS3" s="3" t="inlineStr">
+        <is>
+          <t>1213218</t>
+        </is>
+      </c>
+      <c r="AT3" s="3" t="inlineStr">
+        <is>
+          <t>1411409</t>
+        </is>
+      </c>
+      <c r="AV3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="X3" s="3" t="inlineStr">
+      <c r="AW3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="Y3" s="26" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
-      <c r="Z3" s="26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AA3" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AB3" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AC3" s="26" t="inlineStr">
-        <is>
-          <t>WICK</t>
-        </is>
-      </c>
-      <c r="AD3" s="26" t="inlineStr">
-        <is>
-          <t>WICK</t>
-        </is>
-      </c>
-      <c r="AE3" s="26" t="inlineStr">
-        <is>
-          <t>100.000000%</t>
-        </is>
-      </c>
-      <c r="AF3" s="26" t="inlineStr">
-        <is>
-          <t>100.000000%</t>
-        </is>
-      </c>
-      <c r="AG3" s="26" t="inlineStr">
-        <is>
-          <t>01-Dec-2017</t>
-        </is>
-      </c>
-      <c r="AH3" s="26" t="inlineStr">
-        <is>
-          <t>15-Dec-2017</t>
-        </is>
-      </c>
-      <c r="AI3" s="26" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
-      <c r="AJ3" s="26" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="AK3" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AL3" s="26" t="inlineStr">
-        <is>
-          <t>FLOAT</t>
-        </is>
-      </c>
-      <c r="AM3" s="26" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank Australia - DBU</t>
-        </is>
-      </c>
-      <c r="AN3" s="26" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank Australia - DBU</t>
-        </is>
-      </c>
-      <c r="AO3" s="26" t="inlineStr">
-        <is>
-          <t>OL</t>
-        </is>
-      </c>
-      <c r="AP3" s="26" t="inlineStr">
-        <is>
-          <t>OL</t>
-        </is>
-      </c>
-      <c r="AQ3" s="3" t="inlineStr">
-        <is>
-          <t>1213218</t>
-        </is>
-      </c>
-      <c r="AR3" s="3" t="inlineStr">
-        <is>
-          <t>1213218</t>
-        </is>
-      </c>
-      <c r="AS3" s="3" t="inlineStr">
-        <is>
-          <t>1411409</t>
-        </is>
-      </c>
-      <c r="AU3" s="3" t="inlineStr">
+      <c r="AX3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
       </c>
-      <c r="AV3" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
-      </c>
-      <c r="AW3" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
-        </is>
-      </c>
-      <c r="AX3" s="3" t="inlineStr">
+      <c r="AY3" s="3" t="inlineStr">
         <is>
           <t>1213044</t>
         </is>
@@ -11991,7 +12013,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -12104,7 +12126,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -12217,7 +12239,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -12321,7 +12343,7 @@
       <c r="A5" s="40" t="n"/>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -12339,7 +12361,7 @@
       <c r="A6" s="40" t="n"/>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -12357,7 +12379,7 @@
       <c r="A7" s="40" t="n"/>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>UAT1_18112019165520</t>
+          <t>UAT1_26082020152139</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">

</xml_diff>

<commit_message>
data set updates for outstandingss
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32085" yWindow="2505" windowWidth="18750" windowHeight="12195" tabRatio="955" firstSheet="5" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="955" firstSheet="7" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPR06_LoanMerge" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1253,8 +1253,8 @@
   </sheetPr>
   <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -2224,62 +2224,10 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
-    </row>
     <row r="13">
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
       <c r="AA13" s="80" t="n"/>
     </row>
-    <row r="14">
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
-    </row>
     <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>UAT1_21092020204705</t>
-        </is>
-      </c>
       <c r="Z15" s="79" t="n"/>
     </row>
   </sheetData>
@@ -3640,7 +3588,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>60000030</t>
+          <t>60000006</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
@@ -4247,8 +4195,8 @@
   </sheetPr>
   <dimension ref="A1:BI5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -4266,14 +4214,15 @@
     <col width="31" customWidth="1" style="57" min="11" max="11"/>
     <col width="24.109375" customWidth="1" style="57" min="12" max="12"/>
     <col width="15.88671875" customWidth="1" style="57" min="13" max="13"/>
-    <col width="23" customWidth="1" style="36" min="14" max="14"/>
+    <col width="27.21875" bestFit="1" customWidth="1" style="36" min="14" max="14"/>
     <col width="31.6640625" customWidth="1" style="57" min="15" max="15"/>
     <col width="32.33203125" customWidth="1" style="57" min="16" max="16"/>
     <col width="15.6640625" customWidth="1" style="57" min="17" max="17"/>
     <col width="11" customWidth="1" style="57" min="18" max="18"/>
     <col width="20.88671875" customWidth="1" style="57" min="19" max="19"/>
     <col width="23.6640625" customWidth="1" style="57" min="20" max="20"/>
-    <col width="19.109375" customWidth="1" style="3" min="21" max="22"/>
+    <col width="34.33203125" bestFit="1" customWidth="1" style="3" min="21" max="21"/>
+    <col width="24.21875" customWidth="1" style="3" min="22" max="22"/>
     <col width="27.6640625" customWidth="1" style="3" min="23" max="23"/>
     <col width="29.33203125" customWidth="1" style="3" min="24" max="24"/>
     <col width="27.6640625" customWidth="1" style="3" min="25" max="26"/>
@@ -4463,7 +4412,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>60000732</t>
+          <t>60000004</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4497,9 +4446,9 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="N2" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="O2" s="3" t="inlineStr">
@@ -4509,7 +4458,7 @@
       </c>
       <c r="P2" s="3" t="inlineStr">
         <is>
-          <t>RTGSAUD1-1304</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Q2" s="36" t="inlineStr">
@@ -4527,29 +4476,29 @@
           <t>165</t>
         </is>
       </c>
-      <c r="T2" s="3" t="inlineStr">
-        <is>
-          <t>CUSTLEGAL12130</t>
+      <c r="T2" s="1" t="inlineStr">
+        <is>
+          <t>SanseeraElectronicsLtd</t>
         </is>
       </c>
       <c r="U2" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT04114</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="V2" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT16107</t>
-        </is>
-      </c>
-      <c r="W2" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-5940</t>
-        </is>
-      </c>
-      <c r="X2" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-1655</t>
+          <t>BAN BANK</t>
+        </is>
+      </c>
+      <c r="W2" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="X2" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Y2" s="3" t="inlineStr">
@@ -4562,10 +4511,8 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AA2" s="3" t="inlineStr">
-        <is>
-          <t>33.68</t>
-        </is>
+      <c r="AA2" s="39" t="n">
+        <v>33.68</v>
       </c>
       <c r="AB2" s="3" t="inlineStr">
         <is>
@@ -4642,7 +4589,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>60000733</t>
+          <t>60000005</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -4676,9 +4623,9 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="N3" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="O3" s="3" t="inlineStr">
@@ -4688,7 +4635,7 @@
       </c>
       <c r="P3" s="3" t="inlineStr">
         <is>
-          <t>RTGSAUD1-1304</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Q3" s="36" t="inlineStr">
@@ -4706,29 +4653,29 @@
           <t>165</t>
         </is>
       </c>
-      <c r="T3" s="3" t="inlineStr">
-        <is>
-          <t>CUSTLEGAL12130</t>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>SanseeraElectronicsLtd</t>
         </is>
       </c>
       <c r="U3" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT04114</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="V3" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT16107</t>
-        </is>
-      </c>
-      <c r="W3" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-5940</t>
-        </is>
-      </c>
-      <c r="X3" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-1655</t>
+          <t>BAN BANK</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Y3" s="3" t="inlineStr">
@@ -4741,10 +4688,8 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AA3" s="3" t="inlineStr">
-        <is>
-          <t>33.68</t>
-        </is>
+      <c r="AA3" s="39" t="n">
+        <v>33.68</v>
       </c>
       <c r="AB3" s="3" t="inlineStr">
         <is>
@@ -4821,7 +4766,7 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>60000015</t>
+          <t>60000006</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
@@ -4855,9 +4800,9 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="N4" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
+      <c r="N4" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="O4" s="3" t="inlineStr">
@@ -4867,7 +4812,7 @@
       </c>
       <c r="P4" s="3" t="inlineStr">
         <is>
-          <t>RTGSAUD1-1304</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Q4" s="36" t="inlineStr">
@@ -4885,29 +4830,29 @@
           <t>165</t>
         </is>
       </c>
-      <c r="T4" s="3" t="inlineStr">
-        <is>
-          <t>CUSTLEGAL12130</t>
+      <c r="T4" s="1" t="inlineStr">
+        <is>
+          <t>SanseeraElectronicsLtd</t>
         </is>
       </c>
       <c r="U4" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT04114</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="V4" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT16107</t>
-        </is>
-      </c>
-      <c r="W4" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-5940</t>
-        </is>
-      </c>
-      <c r="X4" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-1655</t>
+          <t>BAN BANK</t>
+        </is>
+      </c>
+      <c r="W4" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="X4" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Y4" s="3" t="inlineStr">
@@ -4920,10 +4865,8 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AA4" s="3" t="inlineStr">
-        <is>
-          <t>94.8</t>
-        </is>
+      <c r="AA4" s="39" t="n">
+        <v>94.8</v>
       </c>
       <c r="AB4" s="3" t="inlineStr">
         <is>
@@ -5030,9 +4973,9 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="N5" s="3" t="inlineStr">
-        <is>
-          <t>1213044</t>
+      <c r="N5" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="O5" s="3" t="inlineStr">
@@ -5042,7 +4985,7 @@
       </c>
       <c r="P5" s="3" t="inlineStr">
         <is>
-          <t>RTGSAUD1-1304</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Q5" s="36" t="inlineStr">
@@ -5060,29 +5003,29 @@
           <t>165</t>
         </is>
       </c>
-      <c r="T5" s="3" t="inlineStr">
-        <is>
-          <t>CUSTLEGAL12130</t>
+      <c r="T5" s="1" t="inlineStr">
+        <is>
+          <t>SanseeraElectronicsLtd</t>
         </is>
       </c>
       <c r="U5" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT04114</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="V5" s="36" t="inlineStr">
         <is>
-          <t>LENDSHORT16107</t>
-        </is>
-      </c>
-      <c r="W5" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-5940</t>
-        </is>
-      </c>
-      <c r="X5" s="3" t="inlineStr">
-        <is>
-          <t>RTGSAUD1-1655</t>
+          <t>BAN BANK</t>
+        </is>
+      </c>
+      <c r="W5" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
+        </is>
+      </c>
+      <c r="X5" s="1" t="inlineStr">
+        <is>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="Y5" s="3" t="inlineStr">
@@ -5095,10 +5038,8 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="AA5" s="3" t="inlineStr">
-        <is>
-          <t>94.8</t>
-        </is>
+      <c r="AA5" s="39" t="n">
+        <v>88.13333333333333</v>
       </c>
       <c r="AB5" s="3" t="inlineStr">
         <is>
@@ -8133,8 +8074,8 @@
   </sheetPr>
   <dimension ref="A1:CI3"/>
   <sheetViews>
-    <sheetView topLeftCell="BN1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BR16" sqref="BR16"/>
+    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -9186,8 +9127,8 @@
   </sheetPr>
   <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -9908,8 +9849,8 @@
   </sheetPr>
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -11958,7 +11899,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -12085,8 +12026,8 @@
   </sheetPr>
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -12284,12 +12225,12 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>60000732</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>SanseeraElectronicsLtd</t>
+          <t>60000004</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
@@ -12304,15 +12245,15 @@
       </c>
       <c r="I2" s="36" t="inlineStr">
         <is>
-          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="J2" s="36" t="inlineStr">
         <is>
-          <t>BIG W BANK</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
+          <t>BAN BANK</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>RTGSAUD1-5940</t>
         </is>
@@ -12324,7 +12265,7 @@
       </c>
       <c r="M2" s="3" t="inlineStr">
         <is>
-          <t>DDA</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="N2" s="3" t="inlineStr">
@@ -12338,7 +12279,7 @@
         </is>
       </c>
       <c r="P2" s="39" t="n">
-        <v>37.5</v>
+        <v>33.68</v>
       </c>
       <c r="Q2" s="3" t="inlineStr">
         <is>
@@ -12365,14 +12306,14 @@
           <t>80,000,000.00</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
+      <c r="V2" s="76" t="inlineStr">
+        <is>
+          <t>28-Nov-2018</t>
+        </is>
+      </c>
+      <c r="W2" s="76" t="inlineStr">
+        <is>
+          <t>31-Aug-2021</t>
         </is>
       </c>
       <c r="X2" s="3" t="inlineStr">
@@ -12419,12 +12360,12 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>60000733</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>SanseeraElectronicsLtd</t>
+          <t>60000005</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -12439,12 +12380,12 @@
       </c>
       <c r="I3" s="36" t="inlineStr">
         <is>
-          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="J3" s="36" t="inlineStr">
         <is>
-          <t>BIG W BANK</t>
+          <t>BAN BANK</t>
         </is>
       </c>
       <c r="K3" s="3" t="inlineStr">
@@ -12459,7 +12400,7 @@
       </c>
       <c r="M3" s="3" t="inlineStr">
         <is>
-          <t>DDA</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="N3" s="3" t="inlineStr">
@@ -12473,7 +12414,7 @@
         </is>
       </c>
       <c r="P3" s="39" t="n">
-        <v>37.5</v>
+        <v>33.68</v>
       </c>
       <c r="Q3" s="3" t="inlineStr">
         <is>
@@ -12500,14 +12441,14 @@
           <t>200,000,000.00</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
+      <c r="V3" s="76" t="inlineStr">
+        <is>
+          <t>28-Nov-2018</t>
+        </is>
+      </c>
+      <c r="W3" s="76" t="inlineStr">
+        <is>
+          <t>31-Aug-2021</t>
         </is>
       </c>
       <c r="X3" s="3" t="inlineStr">
@@ -12554,12 +12495,12 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>60000015</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>SanseeraElectronicsLtd</t>
+          <t>60000006</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
@@ -12574,12 +12515,12 @@
       </c>
       <c r="I4" s="36" t="inlineStr">
         <is>
-          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="J4" s="36" t="inlineStr">
         <is>
-          <t>BIG W BANK</t>
+          <t>BAN BANK</t>
         </is>
       </c>
       <c r="K4" s="3" t="inlineStr">
@@ -12594,7 +12535,7 @@
       </c>
       <c r="M4" s="3" t="inlineStr">
         <is>
-          <t>DDA</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="N4" s="3" t="inlineStr">
@@ -12608,7 +12549,7 @@
         </is>
       </c>
       <c r="P4" s="39" t="n">
-        <v>50</v>
+        <v>94.8</v>
       </c>
       <c r="Q4" s="3" t="inlineStr">
         <is>
@@ -12630,14 +12571,14 @@
           <t>10,000,000.00</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
+      <c r="V4" s="76" t="inlineStr">
+        <is>
+          <t>28-Nov-2018</t>
+        </is>
+      </c>
+      <c r="W4" s="76" t="inlineStr">
+        <is>
+          <t>31-Aug-2021</t>
         </is>
       </c>
       <c r="X4" s="3" t="inlineStr">
@@ -12687,9 +12628,9 @@
           <t>60000018</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>SanseeraElectronicsLtd</t>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>SANSEERAELECTRONICSLTD</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
@@ -12704,12 +12645,12 @@
       </c>
       <c r="I5" s="36" t="inlineStr">
         <is>
-          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+          <t>BIG W BANK</t>
         </is>
       </c>
       <c r="J5" s="36" t="inlineStr">
         <is>
-          <t>BIG W BANK</t>
+          <t>BAN BANK</t>
         </is>
       </c>
       <c r="K5" s="3" t="inlineStr">
@@ -12724,7 +12665,7 @@
       </c>
       <c r="M5" s="3" t="inlineStr">
         <is>
-          <t>DDA</t>
+          <t>RTGS</t>
         </is>
       </c>
       <c r="N5" s="3" t="inlineStr">
@@ -12738,7 +12679,7 @@
         </is>
       </c>
       <c r="P5" s="39" t="n">
-        <v>50</v>
+        <v>88.13333333333333</v>
       </c>
       <c r="Q5" s="3" t="inlineStr">
         <is>
@@ -12760,14 +12701,14 @@
           <t>15,000,000.00</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>31-Aug-2018</t>
+      <c r="V5" s="76" t="inlineStr">
+        <is>
+          <t>28-Nov-2018</t>
+        </is>
+      </c>
+      <c r="W5" s="76" t="inlineStr">
+        <is>
+          <t>31-Aug-2021</t>
         </is>
       </c>
       <c r="X5" s="3" t="inlineStr">
@@ -12823,7 +12764,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N11" sqref="N11"/>
+      <selection pane="topRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>

</xml_diff>

<commit_message>
update steps and data
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CE3804-96F6-46B0-9EE9-94C82F6ED014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB716F9-85C9-412B-8D0A-0339A7D74B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="955" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32775" yWindow="3480" windowWidth="21600" windowHeight="12675" tabRatio="955" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="851">
   <si>
     <t>rowid</t>
   </si>
@@ -2284,9 +2284,6 @@
     <t>14-Feb-2019</t>
   </si>
   <si>
-    <t>20,000,000.00</t>
-  </si>
-  <si>
     <t>BBSY - Bid Loan</t>
   </si>
   <si>
@@ -2329,9 +2326,6 @@
     <t>94.8</t>
   </si>
   <si>
-    <t>CUSTLEGAL11107</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -2597,6 +2591,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>60000007</t>
   </si>
 </sst>
 </file>
@@ -2798,7 +2795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2948,6 +2945,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3670,8 +3670,8 @@
   </sheetPr>
   <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3689,7 +3689,7 @@
     <col min="11" max="11" width="22.88671875" style="23" customWidth="1"/>
     <col min="12" max="12" width="39.88671875" style="23" customWidth="1"/>
     <col min="13" max="13" width="20.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.6640625" style="3" customWidth="1"/>
     <col min="16" max="16" width="29.33203125" style="3" customWidth="1"/>
     <col min="17" max="17" width="17.109375" style="3" customWidth="1"/>
@@ -5018,8 +5018,8 @@
   </sheetPr>
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5046,7 +5046,7 @@
     <col min="26" max="26" width="18.6640625" style="23" customWidth="1"/>
     <col min="27" max="27" width="22.6640625" style="3" customWidth="1"/>
     <col min="28" max="28" width="14.6640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="20.88671875" style="23" customWidth="1"/>
+    <col min="29" max="29" width="27.21875" style="23" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="19.109375" style="3" customWidth="1"/>
     <col min="32" max="32" width="22.109375" style="23" customWidth="1"/>
     <col min="33" max="33" width="23.109375" style="23" customWidth="1"/>
@@ -5178,8 +5178,8 @@
       <c r="C2" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>744</v>
+      <c r="D2" s="85" t="s">
+        <v>601</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>464</v>
@@ -5190,14 +5190,14 @@
       <c r="G2" s="51" t="s">
         <v>746</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="85" t="s">
+        <v>620</v>
+      </c>
+      <c r="I2" s="85" t="s">
+        <v>606</v>
+      </c>
+      <c r="J2" s="51" t="s">
         <v>747</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>612</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>748</v>
       </c>
       <c r="K2" s="51" t="s">
         <v>41</v>
@@ -5206,31 +5206,31 @@
         <v>670</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>41</v>
       </c>
       <c r="O2" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="P2" s="51" t="s">
         <v>750</v>
       </c>
-      <c r="P2" s="51" t="s">
+      <c r="Q2" s="51" t="s">
         <v>751</v>
       </c>
-      <c r="Q2" s="51" t="s">
+      <c r="R2" s="23" t="s">
         <v>752</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>753</v>
       </c>
       <c r="S2" s="23" t="s">
         <v>228</v>
       </c>
       <c r="T2" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>754</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>755</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>605</v>
@@ -5239,40 +5239,40 @@
         <v>671</v>
       </c>
       <c r="X2" s="23" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="Y2" s="23" t="s">
         <v>609</v>
       </c>
       <c r="Z2" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="23" t="s">
         <v>757</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>758</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>46</v>
+      <c r="AC2" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="AD2" s="36" t="s">
-        <v>759</v>
+        <v>500</v>
       </c>
       <c r="AE2" s="36" t="s">
-        <v>760</v>
+        <v>501</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>225</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>602</v>
+        <v>225</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>603</v>
+        <v>225</v>
       </c>
       <c r="AJ2" s="3" t="s">
         <v>225</v>
@@ -5291,8 +5291,8 @@
       <c r="C3" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>614</v>
+      <c r="D3" s="85" t="s">
+        <v>850</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>373</v>
@@ -5306,11 +5306,11 @@
       <c r="H3" s="51" t="s">
         <v>616</v>
       </c>
-      <c r="I3" s="51" t="s">
-        <v>612</v>
+      <c r="I3" s="85" t="s">
+        <v>606</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>41</v>
@@ -5319,28 +5319,28 @@
         <v>670</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="N3" s="23" t="s">
         <v>41</v>
       </c>
       <c r="O3" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="P3" s="51" t="s">
         <v>750</v>
       </c>
-      <c r="P3" s="51" t="s">
+      <c r="Q3" s="51" t="s">
         <v>751</v>
       </c>
-      <c r="Q3" s="51" t="s">
+      <c r="R3" s="23" t="s">
         <v>752</v>
-      </c>
-      <c r="R3" s="23" t="s">
-        <v>753</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>228</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>615</v>
@@ -5349,40 +5349,40 @@
         <v>671</v>
       </c>
       <c r="X3" s="23" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="Y3" s="23" t="s">
         <v>609</v>
       </c>
       <c r="Z3" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="23" t="s">
         <v>757</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="AB3" s="23" t="s">
-        <v>758</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>46</v>
+      <c r="AC3" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="AD3" s="36" t="s">
-        <v>759</v>
+        <v>500</v>
       </c>
       <c r="AE3" s="36" t="s">
-        <v>760</v>
+        <v>501</v>
       </c>
       <c r="AF3" s="3" t="s">
         <v>225</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>602</v>
+        <v>225</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>603</v>
+        <v>225</v>
       </c>
       <c r="AJ3" s="3" t="s">
         <v>225</v>
@@ -5394,7 +5394,7 @@
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5459,10 +5459,10 @@
         <v>286</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F1" s="54" t="s">
         <v>288</v>
@@ -5474,7 +5474,7 @@
         <v>586</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="J1" s="45" t="s">
         <v>656</v>
@@ -5495,13 +5495,13 @@
         <v>585</v>
       </c>
       <c r="P1" s="28" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>665</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="S1" s="54" t="s">
         <v>655</v>
@@ -5510,10 +5510,10 @@
         <v>78</v>
       </c>
       <c r="U1" s="28" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="V1" s="28" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="W1" s="45" t="s">
         <v>741</v>
@@ -5522,25 +5522,25 @@
         <v>738</v>
       </c>
       <c r="Y1" s="45" t="s">
+        <v>768</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>769</v>
+      </c>
+      <c r="AA1" s="26" t="s">
         <v>770</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>771</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>772</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>773</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>774</v>
       </c>
       <c r="AD1" s="46" t="s">
         <v>291</v>
       </c>
       <c r="AE1" s="46" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="AF1" s="46" t="s">
         <v>198</v>
@@ -5549,7 +5549,7 @@
         <v>654</v>
       </c>
       <c r="AH1" s="45" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="AI1" s="45" t="s">
         <v>587</v>
@@ -5575,25 +5575,25 @@
         <v>469</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>464</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>390</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="J2" s="36" t="s">
+        <v>758</v>
+      </c>
+      <c r="K2" s="36" t="s">
         <v>759</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>760</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>602</v>
@@ -5615,10 +5615,10 @@
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="23" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>550</v>
@@ -5630,28 +5630,28 @@
         <v>228</v>
       </c>
       <c r="X2" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="Y2" s="8" t="s">
         <v>757</v>
       </c>
-      <c r="Y2" s="8" t="s">
-        <v>758</v>
-      </c>
       <c r="Z2" s="23" t="s">
+        <v>779</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>780</v>
+      </c>
+      <c r="AB2" s="23" t="s">
         <v>781</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AC2" s="55" t="s">
         <v>782</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>783</v>
-      </c>
-      <c r="AC2" s="55" t="s">
-        <v>784</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>46</v>
       </c>
       <c r="AE2" s="23" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>225</v>
@@ -5660,16 +5660,16 @@
         <v>377</v>
       </c>
       <c r="AH2" s="23" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -5705,7 +5705,7 @@
     <col min="11" max="11" width="31" style="57" customWidth="1"/>
     <col min="12" max="12" width="24.109375" style="57" customWidth="1"/>
     <col min="13" max="13" width="15.88671875" style="57" customWidth="1"/>
-    <col min="14" max="14" width="27.21875" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" style="36" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="31.6640625" style="57" customWidth="1"/>
     <col min="16" max="16" width="32.33203125" style="57" customWidth="1"/>
     <col min="17" max="17" width="15.6640625" style="57" customWidth="1"/>
@@ -5713,7 +5713,7 @@
     <col min="19" max="19" width="20.88671875" style="57" customWidth="1"/>
     <col min="20" max="20" width="23.6640625" style="57" customWidth="1"/>
     <col min="21" max="21" width="34.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.21875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="24.33203125" style="3" customWidth="1"/>
     <col min="23" max="23" width="27.6640625" style="3" customWidth="1"/>
     <col min="24" max="24" width="29.33203125" style="3" customWidth="1"/>
     <col min="25" max="26" width="27.6640625" style="3" customWidth="1"/>
@@ -5737,7 +5737,7 @@
         <v>288</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F1" s="58" t="s">
         <v>578</v>
@@ -5746,19 +5746,19 @@
         <v>703</v>
       </c>
       <c r="H1" s="34" t="s">
+        <v>786</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>787</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>765</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>788</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="L1" s="56" t="s">
         <v>789</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>767</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>790</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>791</v>
       </c>
       <c r="M1" s="56" t="s">
         <v>586</v>
@@ -5776,13 +5776,13 @@
         <v>738</v>
       </c>
       <c r="R1" s="56" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="S1" s="30" t="s">
         <v>527</v>
       </c>
       <c r="T1" s="58" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="U1" s="45" t="s">
         <v>656</v>
@@ -5812,7 +5812,7 @@
         <v>589</v>
       </c>
       <c r="AD1" s="56" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="2" spans="1:61" s="36" customFormat="1" x14ac:dyDescent="0.3">
@@ -5844,11 +5844,11 @@
         <v>606</v>
       </c>
       <c r="J2" s="52" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="K2" s="52"/>
       <c r="L2" s="57" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M2" s="60" t="s">
         <v>390</v>
@@ -5869,7 +5869,7 @@
         <v>716</v>
       </c>
       <c r="S2" s="57" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>212</v>
@@ -5956,7 +5956,7 @@
         <v>611</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="H3" s="52" t="s">
         <v>612</v>
@@ -5965,11 +5965,11 @@
         <v>612</v>
       </c>
       <c r="J3" s="52" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="K3" s="52"/>
       <c r="L3" s="57" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M3" s="60" t="s">
         <v>390</v>
@@ -5990,7 +5990,7 @@
         <v>716</v>
       </c>
       <c r="S3" s="57" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>212</v>
@@ -6077,7 +6077,7 @@
         <v>614</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H4" s="52" t="s">
         <v>616</v>
@@ -6086,11 +6086,11 @@
         <v>616</v>
       </c>
       <c r="J4" s="52" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="K4" s="52"/>
       <c r="L4" s="57" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>390</v>
@@ -6108,10 +6108,10 @@
         <v>228</v>
       </c>
       <c r="R4" s="61" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="S4" s="57" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>212</v>
@@ -6196,7 +6196,7 @@
         <v>619</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H5" s="52" t="s">
         <v>620</v>
@@ -6205,11 +6205,11 @@
         <v>620</v>
       </c>
       <c r="J5" s="52" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="K5" s="52"/>
       <c r="L5" s="57" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M5" s="60" t="s">
         <v>390</v>
@@ -6227,10 +6227,10 @@
         <v>228</v>
       </c>
       <c r="R5" s="61" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="S5" s="57" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>212</v>
@@ -6460,49 +6460,49 @@
         <v>286</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>288</v>
       </c>
       <c r="F1" s="62" t="s">
+        <v>804</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>805</v>
+      </c>
+      <c r="H1" s="62" t="s">
         <v>806</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="I1" s="62" t="s">
         <v>807</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="J1" s="62" t="s">
         <v>808</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="K1" s="62" t="s">
         <v>809</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="L1" s="62" t="s">
         <v>810</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="M1" s="62" t="s">
         <v>811</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="N1" s="62" t="s">
+        <v>789</v>
+      </c>
+      <c r="O1" s="62" t="s">
         <v>812</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="P1" s="62" t="s">
         <v>813</v>
-      </c>
-      <c r="N1" s="62" t="s">
-        <v>791</v>
-      </c>
-      <c r="O1" s="62" t="s">
-        <v>814</v>
-      </c>
-      <c r="P1" s="62" t="s">
-        <v>815</v>
       </c>
       <c r="Q1" s="62" t="s">
         <v>586</v>
       </c>
       <c r="R1" s="62" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="S1" s="65" t="s">
         <v>291</v>
@@ -6514,7 +6514,7 @@
         <v>298</v>
       </c>
       <c r="V1" s="65" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="W1" s="65" t="s">
         <v>656</v>
@@ -6538,46 +6538,46 @@
         <v>738</v>
       </c>
       <c r="AD1" s="62" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="AE1" s="62" t="s">
+        <v>815</v>
+      </c>
+      <c r="AF1" s="62" t="s">
+        <v>816</v>
+      </c>
+      <c r="AG1" s="62" t="s">
         <v>817</v>
       </c>
-      <c r="AF1" s="62" t="s">
+      <c r="AH1" s="62" t="s">
         <v>818</v>
       </c>
-      <c r="AG1" s="62" t="s">
+      <c r="AI1" s="62" t="s">
         <v>819</v>
       </c>
-      <c r="AH1" s="62" t="s">
+      <c r="AJ1" s="62" t="s">
         <v>820</v>
       </c>
-      <c r="AI1" s="62" t="s">
+      <c r="AK1" s="62" t="s">
         <v>821</v>
       </c>
-      <c r="AJ1" s="62" t="s">
+      <c r="AL1" s="62" t="s">
         <v>822</v>
       </c>
-      <c r="AK1" s="62" t="s">
+      <c r="AM1" s="62" t="s">
         <v>823</v>
       </c>
-      <c r="AL1" s="62" t="s">
+      <c r="AN1" s="62" t="s">
         <v>824</v>
       </c>
-      <c r="AM1" s="62" t="s">
+      <c r="AO1" s="62" t="s">
         <v>825</v>
       </c>
-      <c r="AN1" s="62" t="s">
+      <c r="AP1" s="62" t="s">
         <v>826</v>
       </c>
-      <c r="AO1" s="62" t="s">
+      <c r="AQ1" s="62" t="s">
         <v>827</v>
-      </c>
-      <c r="AP1" s="62" t="s">
-        <v>828</v>
-      </c>
-      <c r="AQ1" s="62" t="s">
-        <v>829</v>
       </c>
       <c r="AR1" s="6" t="s">
         <v>599</v>
@@ -6586,7 +6586,7 @@
         <v>596</v>
       </c>
       <c r="AT1" s="62" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="2" spans="1:221" x14ac:dyDescent="0.3">
@@ -6594,7 +6594,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>371</v>
@@ -6606,43 +6606,43 @@
         <v>464</v>
       </c>
       <c r="F2" s="66" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="I2" s="64" t="s">
         <v>831</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="66" t="s">
         <v>832</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>798</v>
-      </c>
-      <c r="I2" s="64" t="s">
-        <v>833</v>
-      </c>
-      <c r="J2" s="66" t="s">
-        <v>834</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>606</v>
       </c>
       <c r="L2" s="64" t="s">
+        <v>833</v>
+      </c>
+      <c r="M2" s="64" t="s">
+        <v>834</v>
+      </c>
+      <c r="N2" s="63" t="s">
+        <v>794</v>
+      </c>
+      <c r="O2" s="64" t="s">
         <v>835</v>
       </c>
-      <c r="M2" s="64" t="s">
+      <c r="P2" s="63" t="s">
         <v>836</v>
-      </c>
-      <c r="N2" s="63" t="s">
-        <v>796</v>
-      </c>
-      <c r="O2" s="64" t="s">
-        <v>837</v>
-      </c>
-      <c r="P2" s="63" t="s">
-        <v>838</v>
       </c>
       <c r="Q2" s="63" t="s">
         <v>390</v>
       </c>
       <c r="R2" s="63" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>46</v>
@@ -6654,13 +6654,13 @@
         <v>377</v>
       </c>
       <c r="V2" s="64" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="W2" s="36" t="s">
+        <v>758</v>
+      </c>
+      <c r="X2" s="36" t="s">
         <v>759</v>
-      </c>
-      <c r="X2" s="36" t="s">
-        <v>760</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>602</v>
@@ -6678,37 +6678,37 @@
         <v>228</v>
       </c>
       <c r="AD2" s="63" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AF2" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AG2" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AH2" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AI2" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AJ2" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AO2" s="3" t="s">
         <v>604</v>
@@ -6726,214 +6726,214 @@
         <v>716</v>
       </c>
       <c r="AT2" s="63" t="s">
+        <v>841</v>
+      </c>
+      <c r="EW2" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="EX2" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="EY2" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="EZ2" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="FA2" s="64" t="s">
         <v>843</v>
       </c>
-      <c r="EW2" s="64" t="s">
+      <c r="FB2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FC2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FD2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FE2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FF2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FG2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FH2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FI2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FJ2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FK2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FL2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FM2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FN2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FO2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FP2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FQ2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FR2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FS2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FT2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FU2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FV2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FW2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FX2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FY2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FZ2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GA2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GB2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GC2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GD2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GE2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GF2" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GG2" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="EX2" s="64" t="s">
+      <c r="GH2" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="EY2" s="64" t="s">
+      <c r="GI2" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="EZ2" s="64" t="s">
+      <c r="GJ2" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="FA2" s="64" t="s">
+      <c r="GK2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GL2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GM2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GN2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GO2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GP2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GQ2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GR2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GS2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GT2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GU2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GV2" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GW2" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FB2" s="64" t="s">
+      <c r="GX2" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FC2" s="64" t="s">
+      <c r="GY2" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FD2" s="64" t="s">
+      <c r="GZ2" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FE2" s="64" t="s">
+      <c r="HA2" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FF2" s="64" t="s">
+      <c r="HB2" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FG2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FH2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FI2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FJ2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FK2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FL2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FM2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FN2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FO2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FP2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FQ2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FR2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FS2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FT2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FU2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FV2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FW2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FX2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FY2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FZ2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GA2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GB2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GC2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GD2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GE2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GF2" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GG2" s="64" t="s">
+      <c r="HC2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GH2" s="64" t="s">
+      <c r="HD2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GI2" s="64" t="s">
+      <c r="HE2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GJ2" s="64" t="s">
+      <c r="HF2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GK2" s="64" t="s">
+      <c r="HG2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GL2" s="64" t="s">
+      <c r="HH2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GM2" s="64" t="s">
+      <c r="HI2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GN2" s="64" t="s">
+      <c r="HJ2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GO2" s="64" t="s">
+      <c r="HK2" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GP2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GQ2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GR2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GS2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GT2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GU2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GV2" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GW2" s="64" t="s">
+      <c r="HL2" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="GX2" s="64" t="s">
+      <c r="HM2" s="3" t="s">
         <v>847</v>
-      </c>
-      <c r="GY2" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="GZ2" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="HA2" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="HB2" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="HC2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HD2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HE2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HF2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HG2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HH2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HI2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HJ2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HK2" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HL2" s="3" t="s">
-        <v>849</v>
-      </c>
-      <c r="HM2" s="3" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="3" spans="1:221" x14ac:dyDescent="0.3">
@@ -6941,7 +6941,7 @@
         <v>417</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>711</v>
@@ -6953,43 +6953,43 @@
         <v>712</v>
       </c>
       <c r="F3" s="66" t="s">
+        <v>829</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="I3" s="64" t="s">
         <v>831</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="66" t="s">
         <v>832</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="I3" s="64" t="s">
-        <v>833</v>
-      </c>
-      <c r="J3" s="66" t="s">
-        <v>834</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>606</v>
       </c>
       <c r="L3" s="64" t="s">
+        <v>833</v>
+      </c>
+      <c r="M3" s="64" t="s">
+        <v>834</v>
+      </c>
+      <c r="N3" s="63" t="s">
+        <v>794</v>
+      </c>
+      <c r="O3" s="64" t="s">
         <v>835</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="P3" s="63" t="s">
         <v>836</v>
-      </c>
-      <c r="N3" s="63" t="s">
-        <v>796</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>837</v>
-      </c>
-      <c r="P3" s="63" t="s">
-        <v>838</v>
       </c>
       <c r="Q3" s="63" t="s">
         <v>390</v>
       </c>
       <c r="R3" s="63" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>46</v>
@@ -7001,13 +7001,13 @@
         <v>377</v>
       </c>
       <c r="V3" s="64" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="W3" s="36" t="s">
+        <v>758</v>
+      </c>
+      <c r="X3" s="36" t="s">
         <v>759</v>
-      </c>
-      <c r="X3" s="36" t="s">
-        <v>760</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>602</v>
@@ -7025,37 +7025,37 @@
         <v>228</v>
       </c>
       <c r="AD3" s="63" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AF3" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AG3" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AH3" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AI3" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AJ3" s="63" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="AK3" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AO3" s="3" t="s">
         <v>604</v>
@@ -7073,214 +7073,214 @@
         <v>716</v>
       </c>
       <c r="AT3" s="63" t="s">
+        <v>841</v>
+      </c>
+      <c r="EW3" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="EX3" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="EY3" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="EZ3" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="FA3" s="64" t="s">
         <v>843</v>
       </c>
-      <c r="EW3" s="64" t="s">
+      <c r="FB3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FC3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FD3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FE3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FF3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FG3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FH3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FI3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FJ3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FK3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FL3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FM3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FN3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FO3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FP3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FQ3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FR3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FS3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FT3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FU3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FV3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FW3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FX3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FY3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="FZ3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GA3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GB3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GC3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GD3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GE3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GF3" s="64" t="s">
+        <v>843</v>
+      </c>
+      <c r="GG3" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="EX3" s="64" t="s">
+      <c r="GH3" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="EY3" s="64" t="s">
+      <c r="GI3" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="EZ3" s="64" t="s">
+      <c r="GJ3" s="64" t="s">
         <v>844</v>
       </c>
-      <c r="FA3" s="64" t="s">
+      <c r="GK3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GL3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GM3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GN3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GO3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GP3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GQ3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GR3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GS3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GT3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GU3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GV3" s="64" t="s">
+        <v>844</v>
+      </c>
+      <c r="GW3" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FB3" s="64" t="s">
+      <c r="GX3" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FC3" s="64" t="s">
+      <c r="GY3" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FD3" s="64" t="s">
+      <c r="GZ3" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FE3" s="64" t="s">
+      <c r="HA3" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FF3" s="64" t="s">
+      <c r="HB3" s="64" t="s">
         <v>845</v>
       </c>
-      <c r="FG3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FH3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FI3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FJ3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FK3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FL3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FM3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FN3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FO3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FP3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FQ3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FR3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FS3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FT3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FU3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FV3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FW3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FX3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FY3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="FZ3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GA3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GB3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GC3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GD3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GE3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GF3" s="64" t="s">
-        <v>845</v>
-      </c>
-      <c r="GG3" s="64" t="s">
+      <c r="HC3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GH3" s="64" t="s">
+      <c r="HD3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GI3" s="64" t="s">
+      <c r="HE3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GJ3" s="64" t="s">
+      <c r="HF3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GK3" s="64" t="s">
+      <c r="HG3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GL3" s="64" t="s">
+      <c r="HH3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GM3" s="64" t="s">
+      <c r="HI3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GN3" s="64" t="s">
+      <c r="HJ3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GO3" s="64" t="s">
+      <c r="HK3" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="GP3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GQ3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GR3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GS3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GT3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GU3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GV3" s="64" t="s">
-        <v>846</v>
-      </c>
-      <c r="GW3" s="64" t="s">
+      <c r="HL3" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="GX3" s="64" t="s">
+      <c r="HM3" s="3" t="s">
         <v>847</v>
-      </c>
-      <c r="GY3" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="GZ3" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="HA3" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="HB3" s="64" t="s">
-        <v>847</v>
-      </c>
-      <c r="HC3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HD3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HE3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HF3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HG3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HH3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HI3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HJ3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HK3" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="HL3" s="3" t="s">
-        <v>849</v>
-      </c>
-      <c r="HM3" s="3" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="4" spans="1:221" x14ac:dyDescent="0.3">
@@ -7315,7 +7315,7 @@
     </row>
     <row r="10" spans="1:221" x14ac:dyDescent="0.3">
       <c r="G10" s="63" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>46</v>
@@ -9362,8 +9362,8 @@
   </sheetPr>
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10812,8 +10812,8 @@
   </sheetPr>
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10825,7 +10825,7 @@
     <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="34.33203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="18.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" style="3" customWidth="1"/>

</xml_diff>

<commit_message>
update value in datasets
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB716F9-85C9-412B-8D0A-0339A7D74B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156FB924-6CAA-49BE-9D52-E88CDFDAE00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32775" yWindow="3480" windowWidth="21600" windowHeight="12675" tabRatio="955" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="955" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,14 @@
     <sheet name="CRED02_FacilitySetup" sheetId="4" r:id="rId4"/>
     <sheet name="CRED01_Primaries" sheetId="5" r:id="rId5"/>
     <sheet name="CRED08_FacilityFeeSetup" sheetId="6" r:id="rId6"/>
-    <sheet name="CRED01_PricingRule" sheetId="7" r:id="rId7"/>
-    <sheet name="SERV01_LoanDrawdown" sheetId="8" r:id="rId8"/>
+    <sheet name="SERV01_LoanDrawdown" sheetId="7" r:id="rId7"/>
+    <sheet name="CRED01_PricingRule" sheetId="8" r:id="rId8"/>
     <sheet name="CRED09_AdminFee" sheetId="9" r:id="rId9"/>
     <sheet name="SERV29_CommitmentFeePayment" sheetId="10" r:id="rId10"/>
     <sheet name="CRED10_EventFee" sheetId="11" r:id="rId11"/>
-    <sheet name="AMCH04_DealChangeTransaction" sheetId="12" r:id="rId12"/>
-    <sheet name="UAT01_Runbook" sheetId="13" r:id="rId13"/>
-    <sheet name="SERV23_Paperclip" sheetId="14" r:id="rId14"/>
+    <sheet name="SERV23_Paperclip" sheetId="14" r:id="rId12"/>
+    <sheet name="AMCH04_DealChangeTransaction" sheetId="12" r:id="rId13"/>
+    <sheet name="UAT01_Runbook" sheetId="13" r:id="rId14"/>
     <sheet name="SERV40_BreakFunding" sheetId="15" r:id="rId15"/>
     <sheet name="SERV08C_ComprehensiveRepricing" sheetId="16" r:id="rId16"/>
     <sheet name="COMPR06_LoanMerge" sheetId="17" r:id="rId17"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="853">
   <si>
     <t>rowid</t>
   </si>
@@ -1156,13 +1156,13 @@
     <t>UAT1</t>
   </si>
   <si>
-    <t>UAT1_21092020204705</t>
-  </si>
-  <si>
-    <t>UAT121092020204705</t>
-  </si>
-  <si>
-    <t>FACB_21092020215522</t>
+    <t>UAT1_07102020102617</t>
+  </si>
+  <si>
+    <t>UAT107102020102617</t>
+  </si>
+  <si>
+    <t>FACB_07102020113236</t>
   </si>
   <si>
     <t>Sales Group 1</t>
@@ -1435,7 +1435,7 @@
     <t>FACA_</t>
   </si>
   <si>
-    <t>FACA_21092020212204</t>
+    <t>FACA_07102020105538</t>
   </si>
   <si>
     <t>Revolver</t>
@@ -1759,6 +1759,147 @@
     <t>1.350000</t>
   </si>
   <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>Borrower_Name</t>
+  </si>
+  <si>
+    <t>Borrower_RemittanceInstruction</t>
+  </si>
+  <si>
+    <t>Lender2</t>
+  </si>
+  <si>
+    <t>Lender_RemittanceDescription</t>
+  </si>
+  <si>
+    <t>Lender2_RemittanceDescription</t>
+  </si>
+  <si>
+    <t>Lender_RemittanceInstruction</t>
+  </si>
+  <si>
+    <t>Lender2_RemittanceInstruction</t>
+  </si>
+  <si>
+    <t>Pricing_Option</t>
+  </si>
+  <si>
+    <t>HostBank_LenderShare</t>
+  </si>
+  <si>
+    <t>Lender1_Share</t>
+  </si>
+  <si>
+    <t>Lender2_Share</t>
+  </si>
+  <si>
+    <t>Outstanding_Type</t>
+  </si>
+  <si>
+    <t>Outstanding_Currency</t>
+  </si>
+  <si>
+    <t>Loan_RequestedAmount</t>
+  </si>
+  <si>
+    <t>Loan_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Loan_MaturityDate</t>
+  </si>
+  <si>
+    <t>Loan_IntCycleFrequency</t>
+  </si>
+  <si>
+    <t>Loan_BorrowerBaseRate</t>
+  </si>
+  <si>
+    <t>Loan_FacilitySpread</t>
+  </si>
+  <si>
+    <t>Loan_OverrideSpread</t>
+  </si>
+  <si>
+    <t>Loan_RepricingFrequency</t>
+  </si>
+  <si>
+    <t>Establish Outstanding - Deal 1 - Facility A - Outstanding A1</t>
+  </si>
+  <si>
+    <t>60000022</t>
+  </si>
+  <si>
+    <t>RTGSAUD1-5940</t>
+  </si>
+  <si>
+    <t>RTGSAUD1-1655</t>
+  </si>
+  <si>
+    <t>28.9866666666667</t>
+  </si>
+  <si>
+    <t>37.3333333333333</t>
+  </si>
+  <si>
+    <t>80,000,000.00</t>
+  </si>
+  <si>
+    <t>12-Dec-2018</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>2.14</t>
+  </si>
+  <si>
+    <t>1 Months</t>
+  </si>
+  <si>
+    <t>Establish Outstanding - Deal 1 - Facility A - Outstanding A2</t>
+  </si>
+  <si>
+    <t>60000023</t>
+  </si>
+  <si>
+    <t>200,000,000.00</t>
+  </si>
+  <si>
+    <t>Establish Outstanding - Deal 1 - Facility B - Outstanding B1</t>
+  </si>
+  <si>
+    <t>60000024</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>10,000,000.00</t>
+  </si>
+  <si>
+    <t>27-Dec-2018</t>
+  </si>
+  <si>
+    <t>1.78</t>
+  </si>
+  <si>
+    <t>Establish Outstanding - Deal 1 - Facility B - Outstanding B2</t>
+  </si>
+  <si>
+    <t>60000025</t>
+  </si>
+  <si>
+    <t>15,000,000.00</t>
+  </si>
+  <si>
+    <t>10-Jan-2019</t>
+  </si>
+  <si>
+    <t>1.9952</t>
+  </si>
+  <si>
     <t>PricingRule_Fee1</t>
   </si>
   <si>
@@ -1777,138 +1918,6 @@
     <t>AGENCY DEAL ONE</t>
   </si>
   <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
-    <t>Borrower_Name</t>
-  </si>
-  <si>
-    <t>Borrower_RemittanceInstruction</t>
-  </si>
-  <si>
-    <t>Lender2</t>
-  </si>
-  <si>
-    <t>Lender_RemittanceDescription</t>
-  </si>
-  <si>
-    <t>Lender2_RemittanceDescription</t>
-  </si>
-  <si>
-    <t>Lender_RemittanceInstruction</t>
-  </si>
-  <si>
-    <t>Lender2_RemittanceInstruction</t>
-  </si>
-  <si>
-    <t>Pricing_Option</t>
-  </si>
-  <si>
-    <t>HostBank_LenderShare</t>
-  </si>
-  <si>
-    <t>Lender1_Share</t>
-  </si>
-  <si>
-    <t>Lender2_Share</t>
-  </si>
-  <si>
-    <t>Outstanding_Type</t>
-  </si>
-  <si>
-    <t>Outstanding_Currency</t>
-  </si>
-  <si>
-    <t>Loan_RequestedAmount</t>
-  </si>
-  <si>
-    <t>Loan_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Loan_MaturityDate</t>
-  </si>
-  <si>
-    <t>Loan_IntCycleFrequency</t>
-  </si>
-  <si>
-    <t>Loan_BorrowerBaseRate</t>
-  </si>
-  <si>
-    <t>Loan_FacilitySpread</t>
-  </si>
-  <si>
-    <t>Loan_OverrideSpread</t>
-  </si>
-  <si>
-    <t>Loan_RepricingFrequency</t>
-  </si>
-  <si>
-    <t>Establish Outstanding - Deal 1 - Facility A - Outstanding A1</t>
-  </si>
-  <si>
-    <t>60000004</t>
-  </si>
-  <si>
-    <t>RTGSAUD1-5940</t>
-  </si>
-  <si>
-    <t>RTGSAUD1-1655</t>
-  </si>
-  <si>
-    <t>28.9866666666667</t>
-  </si>
-  <si>
-    <t>37.3333333333333</t>
-  </si>
-  <si>
-    <t>80,000,000.00</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>2.14</t>
-  </si>
-  <si>
-    <t>1 Months</t>
-  </si>
-  <si>
-    <t>Establish Outstanding - Deal 1 - Facility A - Outstanding A2</t>
-  </si>
-  <si>
-    <t>60000005</t>
-  </si>
-  <si>
-    <t>200,000,000.00</t>
-  </si>
-  <si>
-    <t>Establish Outstanding - Deal 1 - Facility B - Outstanding B1</t>
-  </si>
-  <si>
-    <t>60000006</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>10,000,000.00</t>
-  </si>
-  <si>
-    <t>1.78</t>
-  </si>
-  <si>
-    <t>Establish Outstanding - Deal 1 - Facility B - Outstanding B2</t>
-  </si>
-  <si>
-    <t>60000018</t>
-  </si>
-  <si>
-    <t>15,000,000.00</t>
-  </si>
-  <si>
-    <t>1.9952</t>
-  </si>
-  <si>
     <t>AdminFee_FlatAmount</t>
   </si>
   <si>
@@ -2071,6 +2080,9 @@
     <t>31-Dec-2018</t>
   </si>
   <si>
+    <t>30-Nov-2018</t>
+  </si>
+  <si>
     <t>31-Jan-2019</t>
   </si>
   <si>
@@ -2275,9 +2287,6 @@
     <t>NoticeStatus</t>
   </si>
   <si>
-    <t>60000022</t>
-  </si>
-  <si>
     <t>Issuance</t>
   </si>
   <si>
@@ -2317,69 +2326,63 @@
     <t>Awaiting release</t>
   </si>
   <si>
+    <t>60000032</t>
+  </si>
+  <si>
+    <t>94.8</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Search_By</t>
+  </si>
+  <si>
+    <t>Legal_Entity</t>
+  </si>
+  <si>
+    <t>Legal_Entity_Amount</t>
+  </si>
+  <si>
+    <t>Loan_TotalGlobalInterest</t>
+  </si>
+  <si>
+    <t>Pricing_Option_From_Breakfunding</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Notice_Status</t>
+  </si>
+  <si>
+    <t>WIP_TransactionType</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingApprovalStatus</t>
+  </si>
+  <si>
+    <t>WIP_OutstandingType</t>
+  </si>
+  <si>
+    <t>WIP_AwaitingReleaseStatus</t>
+  </si>
+  <si>
+    <t>Lender_ShortName</t>
+  </si>
+  <si>
+    <t>Deal/Facility</t>
+  </si>
+  <si>
     <t>LENDSHORT04114</t>
   </si>
   <si>
     <t>LENDSHORT16107</t>
   </si>
   <si>
-    <t>94.8</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Search_By</t>
-  </si>
-  <si>
-    <t>Legal_Entity</t>
-  </si>
-  <si>
-    <t>Legal_Entity_Amount</t>
-  </si>
-  <si>
-    <t>Loan_TotalGlobalInterest</t>
-  </si>
-  <si>
-    <t>Pricing_Option_From_Breakfunding</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Notice_Status</t>
-  </si>
-  <si>
-    <t>WIP_TransactionType</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingApprovalStatus</t>
-  </si>
-  <si>
-    <t>WIP_OutstandingType</t>
-  </si>
-  <si>
-    <t>WIP_AwaitingReleaseStatus</t>
-  </si>
-  <si>
-    <t>Lender_ShortName</t>
-  </si>
-  <si>
-    <t>Deal/Facility</t>
-  </si>
-  <si>
-    <t>06000099</t>
-  </si>
-  <si>
-    <t>COMMONWEALTH BANK AU-DBU</t>
-  </si>
-  <si>
     <t>CB001/Hold for Investment - Australia/NR_COL</t>
   </si>
   <si>
-    <t>RE_RES-Real Estate Solutions</t>
-  </si>
-  <si>
     <t>Payments</t>
   </si>
   <si>
@@ -2431,15 +2434,12 @@
     <t>165</t>
   </si>
   <si>
-    <t>60000026</t>
+    <t>60000028</t>
   </si>
   <si>
     <t>567,780.82</t>
   </si>
   <si>
-    <t>60000030</t>
-  </si>
-  <si>
     <t>25,134.25</t>
   </si>
   <si>
@@ -2593,16 +2593,23 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>60000007</t>
+    <t>20,000,000.00</t>
+  </si>
+  <si>
+    <t>BP_CML-Commercial Lending</t>
+  </si>
+  <si>
+    <t>60000040</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -2795,7 +2802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2946,6 +2953,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3671,7 +3681,7 @@
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:P13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3701,8 +3711,9 @@
     <col min="23" max="23" width="10.6640625" style="3" customWidth="1"/>
     <col min="24" max="24" width="11.33203125" style="3" customWidth="1"/>
     <col min="25" max="25" width="13.5546875" style="3" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" style="3" customWidth="1"/>
-    <col min="27" max="28" width="16.33203125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.109375" style="3" customWidth="1"/>
     <col min="29" max="29" width="9.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3723,13 +3734,13 @@
         <v>288</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="I1" s="45" t="s">
         <v>291</v>
@@ -3738,61 +3749,61 @@
         <v>198</v>
       </c>
       <c r="K1" s="45" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="L1" s="45" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="M1" s="45" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="N1" s="45" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="S1" s="45" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="T1" s="45" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="U1" s="45" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="V1" s="45" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="W1" s="45" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="X1" s="45" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="Y1" s="45" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="Z1" s="45" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="AA1" s="45" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="AB1" s="45" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="AC1" s="45" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3812,13 +3823,13 @@
         <v>464</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>41</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>212</v>
@@ -3830,7 +3841,7 @@
         <v>242</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M2" s="36" t="s">
         <v>500</v>
@@ -3851,7 +3862,7 @@
         <v>225</v>
       </c>
       <c r="S2" s="1">
-        <v>109315.07</v>
+        <v>112958.9</v>
       </c>
       <c r="T2" s="3">
         <v>1.4</v>
@@ -3869,7 +3880,7 @@
         <v>384</v>
       </c>
       <c r="Y2" s="76" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="Z2" s="78">
         <v>33.68000067669842</v>
@@ -3881,7 +3892,7 @@
         <v>37.333333178835993</v>
       </c>
       <c r="AC2" s="23" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3901,13 +3912,13 @@
         <v>373</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>41</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>212</v>
@@ -3916,10 +3927,10 @@
         <v>225</v>
       </c>
       <c r="K3" s="76" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M3" s="36" t="s">
         <v>500</v>
@@ -3943,7 +3954,7 @@
         <v>8219.18</v>
       </c>
       <c r="T3" s="1">
-        <v>0.4</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="U3" s="39">
         <v>25000000</v>
@@ -3958,17 +3969,17 @@
         <v>384</v>
       </c>
       <c r="Y3" s="76" t="s">
-        <v>672</v>
-      </c>
-      <c r="Z3" s="39">
+        <v>675</v>
+      </c>
+      <c r="Z3" s="78">
         <v>94.799967880007486</v>
       </c>
-      <c r="AA3" s="78">
+      <c r="AA3" s="86">
         <v>5.200032119992505</v>
       </c>
       <c r="AB3" s="3"/>
       <c r="AC3" s="23" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3988,13 +3999,13 @@
         <v>464</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>417</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>212</v>
@@ -4006,7 +4017,7 @@
         <v>242</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M4" s="36" t="s">
         <v>500</v>
@@ -4033,7 +4044,7 @@
         <v>1.4</v>
       </c>
       <c r="U4" s="39" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="V4" s="3">
         <v>241835.62</v>
@@ -4041,11 +4052,11 @@
       <c r="W4" s="81">
         <v>365</v>
       </c>
-      <c r="X4" s="76" t="s">
-        <v>384</v>
-      </c>
-      <c r="Y4" s="76" t="s">
-        <v>672</v>
+      <c r="X4" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>679</v>
       </c>
       <c r="Z4" s="78">
         <v>33.68000067669842</v>
@@ -4057,7 +4068,7 @@
         <v>37.333333178835993</v>
       </c>
       <c r="AC4" s="23" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="5" spans="1:29" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4077,13 +4088,13 @@
         <v>373</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>417</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>212</v>
@@ -4092,10 +4103,10 @@
         <v>225</v>
       </c>
       <c r="K5" s="76" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M5" s="36" t="s">
         <v>500</v>
@@ -4116,10 +4127,10 @@
         <v>225</v>
       </c>
       <c r="S5" s="3">
-        <v>5479.45</v>
+        <v>8493.15</v>
       </c>
       <c r="T5" s="1">
-        <v>0.4</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="U5" s="39">
         <v>25000000</v>
@@ -4130,21 +4141,21 @@
       <c r="W5" s="81">
         <v>365</v>
       </c>
-      <c r="X5" s="76" t="s">
-        <v>675</v>
-      </c>
-      <c r="Y5" s="76" t="s">
-        <v>675</v>
-      </c>
-      <c r="Z5" s="39">
-        <v>61.161288803329747</v>
-      </c>
-      <c r="AA5" s="78">
-        <v>3.3548212382920362</v>
+      <c r="X5" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z5" s="78">
+        <v>94.800044741939089</v>
+      </c>
+      <c r="AA5" s="86">
+        <v>5.1999552580609079</v>
       </c>
       <c r="AB5" s="3"/>
       <c r="AC5" s="23" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4164,13 +4175,13 @@
         <v>464</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>511</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>212</v>
@@ -4182,7 +4193,7 @@
         <v>242</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>500</v>
@@ -4217,23 +4228,23 @@
       <c r="W6" s="81">
         <v>365</v>
       </c>
-      <c r="X6" s="76" t="s">
-        <v>676</v>
-      </c>
-      <c r="Y6" s="76" t="s">
-        <v>676</v>
+      <c r="X6" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>678</v>
       </c>
       <c r="Z6" s="78">
         <v>33.68000067669842</v>
       </c>
       <c r="AA6" s="78">
-        <v>28.986666144465609</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>605</v>
+        <v>28.986666831918509</v>
+      </c>
+      <c r="AB6" s="78">
+        <v>37.333330972592691</v>
       </c>
       <c r="AC6" s="23" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="7" spans="1:29" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4253,13 +4264,13 @@
         <v>373</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>511</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>212</v>
@@ -4268,10 +4279,10 @@
         <v>225</v>
       </c>
       <c r="K7" s="76" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="M7" s="36" t="s">
         <v>500</v>
@@ -4306,21 +4317,21 @@
       <c r="W7" s="82">
         <v>365</v>
       </c>
-      <c r="X7" s="76" t="s">
-        <v>676</v>
-      </c>
-      <c r="Y7" s="76" t="s">
-        <v>676</v>
-      </c>
-      <c r="Z7" s="39">
+      <c r="X7" t="s">
+        <v>680</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>678</v>
+      </c>
+      <c r="Z7" s="78">
         <v>94.800044741939089</v>
       </c>
-      <c r="AA7" s="78">
+      <c r="AA7" s="86">
         <v>5.1999552580609079</v>
       </c>
       <c r="AB7" s="3"/>
       <c r="AC7" s="23" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -4493,55 +4504,55 @@
         <v>288</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="P1" s="30" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="Q1" s="30" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="R1" s="30" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="S1" s="30" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="T1" s="30" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="U1" s="30" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="BF1" s="6"/>
       <c r="CN1" s="40"/>
@@ -4605,21 +4616,21 @@
         <v>499</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>577</v>
+        <v>624</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>407</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="I2" s="29"/>
       <c r="J2" s="10"/>
       <c r="K2" s="41" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="L2" s="39"/>
       <c r="M2" s="7"/>
@@ -4627,22 +4638,22 @@
         <v>100</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="P2" s="7">
         <v>2</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="R2" s="42" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="U2" s="11" t="s">
         <v>221</v>
@@ -4669,6 +4680,393 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AK3"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" style="3" customWidth="1"/>
+    <col min="6" max="10" width="23.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="26.44140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="23" style="3" customWidth="1"/>
+    <col min="17" max="18" width="23.6640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" style="3" customWidth="1"/>
+    <col min="21" max="22" width="16.33203125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="40.6640625" style="23" customWidth="1"/>
+    <col min="24" max="24" width="17.5546875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="20.44140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" style="23" customWidth="1"/>
+    <col min="27" max="27" width="22.6640625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="27.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="19.109375" style="3" customWidth="1"/>
+    <col min="32" max="32" width="22.109375" style="23" customWidth="1"/>
+    <col min="33" max="33" width="23.109375" style="23" customWidth="1"/>
+    <col min="34" max="34" width="29.44140625" style="3" customWidth="1"/>
+    <col min="35" max="35" width="29.33203125" style="3" customWidth="1"/>
+    <col min="36" max="37" width="27.6640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="50" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>572</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>654</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>732</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>733</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>580</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>734</v>
+      </c>
+      <c r="L1" s="50" t="s">
+        <v>735</v>
+      </c>
+      <c r="M1" s="50" t="s">
+        <v>736</v>
+      </c>
+      <c r="N1" s="50" t="s">
+        <v>737</v>
+      </c>
+      <c r="O1" s="50" t="s">
+        <v>738</v>
+      </c>
+      <c r="P1" s="50" t="s">
+        <v>739</v>
+      </c>
+      <c r="Q1" s="50" t="s">
+        <v>740</v>
+      </c>
+      <c r="R1" s="50" t="s">
+        <v>741</v>
+      </c>
+      <c r="S1" s="50" t="s">
+        <v>742</v>
+      </c>
+      <c r="T1" s="45" t="s">
+        <v>668</v>
+      </c>
+      <c r="U1" s="45" t="s">
+        <v>669</v>
+      </c>
+      <c r="V1" s="45" t="s">
+        <v>670</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>658</v>
+      </c>
+      <c r="X1" s="50" t="s">
+        <v>743</v>
+      </c>
+      <c r="Y1" s="50" t="s">
+        <v>744</v>
+      </c>
+      <c r="Z1" s="50" t="s">
+        <v>745</v>
+      </c>
+      <c r="AA1" s="50" t="s">
+        <v>746</v>
+      </c>
+      <c r="AB1" s="50" t="s">
+        <v>747</v>
+      </c>
+      <c r="AC1" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD1" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="AE1" s="45" t="s">
+        <v>660</v>
+      </c>
+      <c r="AF1" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="45" t="s">
+        <v>657</v>
+      </c>
+      <c r="AH1" s="45" t="s">
+        <v>576</v>
+      </c>
+      <c r="AI1" s="45" t="s">
+        <v>577</v>
+      </c>
+      <c r="AJ1" s="45" t="s">
+        <v>578</v>
+      </c>
+      <c r="AK1" s="45" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>852</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>748</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>749</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>850</v>
+      </c>
+      <c r="I2" s="83" t="s">
+        <v>607</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>750</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="51" t="s">
+        <v>673</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>752</v>
+      </c>
+      <c r="P2" s="51" t="s">
+        <v>753</v>
+      </c>
+      <c r="Q2" s="51" t="s">
+        <v>754</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>755</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>758</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="23" t="s">
+        <v>760</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD2" s="36" t="s">
+        <v>500</v>
+      </c>
+      <c r="AE2" s="36" t="s">
+        <v>501</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>761</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>748</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>749</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>611</v>
+      </c>
+      <c r="I3" s="83" t="s">
+        <v>607</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>750</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="51" t="s">
+        <v>673</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>752</v>
+      </c>
+      <c r="P3" s="51" t="s">
+        <v>753</v>
+      </c>
+      <c r="Q3" s="51" t="s">
+        <v>754</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>755</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="X3" s="23" t="s">
+        <v>758</v>
+      </c>
+      <c r="Y3" s="23" t="s">
+        <v>604</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="23" t="s">
+        <v>760</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AD3" s="36" t="s">
+        <v>500</v>
+      </c>
+      <c r="AE3" s="36" t="s">
+        <v>501</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4676,7 +5074,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4700,10 +5098,10 @@
         <v>286</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="F1" s="48" t="s">
         <v>316</v>
@@ -4720,7 +5118,7 @@
         <v>371</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>387</v>
@@ -4736,7 +5134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4780,40 +5178,40 @@
         <v>288</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>198</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -4821,22 +5219,22 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="G2" s="73" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>390</v>
@@ -4848,13 +5246,13 @@
         <v>225</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="N2" s="3">
         <v>165</v>
@@ -4868,22 +5266,22 @@
         <v>417</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="G3" s="73" t="s">
         <v>719</v>
-      </c>
-      <c r="G3" s="73" t="s">
-        <v>715</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>390</v>
@@ -4895,13 +5293,13 @@
         <v>225</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="N3" s="3">
         <v>165</v>
@@ -4915,22 +5313,22 @@
         <v>511</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="G4" s="73" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>390</v>
@@ -4942,13 +5340,13 @@
         <v>225</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="N4" s="3">
         <v>165</v>
@@ -4962,22 +5360,22 @@
         <v>551</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>711</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>721</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="G5" s="73" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>390</v>
@@ -4989,13 +5387,13 @@
         <v>225</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c r="N5" s="3">
         <v>165</v>
@@ -5008,393 +5406,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AK3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="3" customWidth="1"/>
-    <col min="6" max="10" width="23.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="19" style="3" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="19.109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="26.44140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="23" style="3" customWidth="1"/>
-    <col min="17" max="18" width="23.6640625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="17.6640625" style="3" customWidth="1"/>
-    <col min="21" max="22" width="16.33203125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="40.6640625" style="23" customWidth="1"/>
-    <col min="24" max="24" width="17.5546875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="20.44140625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="18.6640625" style="23" customWidth="1"/>
-    <col min="27" max="27" width="22.6640625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="14.6640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="27.21875" style="23" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="19.109375" style="3" customWidth="1"/>
-    <col min="32" max="32" width="22.109375" style="23" customWidth="1"/>
-    <col min="33" max="33" width="23.109375" style="23" customWidth="1"/>
-    <col min="34" max="34" width="29.44140625" style="3" customWidth="1"/>
-    <col min="35" max="35" width="29.33203125" style="3" customWidth="1"/>
-    <col min="36" max="37" width="27.6640625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:37" s="50" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>578</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>288</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>651</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>728</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>592</v>
-      </c>
-      <c r="I1" s="50" t="s">
-        <v>729</v>
-      </c>
-      <c r="J1" s="50" t="s">
-        <v>586</v>
-      </c>
-      <c r="K1" s="50" t="s">
-        <v>730</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>731</v>
-      </c>
-      <c r="M1" s="50" t="s">
-        <v>732</v>
-      </c>
-      <c r="N1" s="50" t="s">
-        <v>733</v>
-      </c>
-      <c r="O1" s="50" t="s">
-        <v>734</v>
-      </c>
-      <c r="P1" s="50" t="s">
-        <v>735</v>
-      </c>
-      <c r="Q1" s="50" t="s">
-        <v>736</v>
-      </c>
-      <c r="R1" s="50" t="s">
-        <v>737</v>
-      </c>
-      <c r="S1" s="50" t="s">
-        <v>738</v>
-      </c>
-      <c r="T1" s="45" t="s">
-        <v>665</v>
-      </c>
-      <c r="U1" s="45" t="s">
-        <v>666</v>
-      </c>
-      <c r="V1" s="45" t="s">
-        <v>667</v>
-      </c>
-      <c r="W1" s="28" t="s">
-        <v>655</v>
-      </c>
-      <c r="X1" s="50" t="s">
-        <v>739</v>
-      </c>
-      <c r="Y1" s="50" t="s">
-        <v>740</v>
-      </c>
-      <c r="Z1" s="50" t="s">
-        <v>741</v>
-      </c>
-      <c r="AA1" s="50" t="s">
-        <v>742</v>
-      </c>
-      <c r="AB1" s="50" t="s">
-        <v>743</v>
-      </c>
-      <c r="AC1" s="45" t="s">
-        <v>291</v>
-      </c>
-      <c r="AD1" s="45" t="s">
-        <v>656</v>
-      </c>
-      <c r="AE1" s="45" t="s">
-        <v>657</v>
-      </c>
-      <c r="AF1" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG1" s="45" t="s">
-        <v>654</v>
-      </c>
-      <c r="AH1" s="45" t="s">
-        <v>582</v>
-      </c>
-      <c r="AI1" s="45" t="s">
-        <v>583</v>
-      </c>
-      <c r="AJ1" s="45" t="s">
-        <v>584</v>
-      </c>
-      <c r="AK1" s="45" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="D2" s="85" t="s">
-        <v>601</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>745</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>746</v>
-      </c>
-      <c r="H2" s="85" t="s">
-        <v>620</v>
-      </c>
-      <c r="I2" s="85" t="s">
-        <v>606</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>747</v>
-      </c>
-      <c r="K2" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="51" t="s">
-        <v>670</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>749</v>
-      </c>
-      <c r="P2" s="51" t="s">
-        <v>750</v>
-      </c>
-      <c r="Q2" s="51" t="s">
-        <v>751</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>752</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>753</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>754</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="X2" s="23" t="s">
-        <v>755</v>
-      </c>
-      <c r="Y2" s="23" t="s">
-        <v>609</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>756</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="23" t="s">
-        <v>757</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="AD2" s="36" t="s">
-        <v>500</v>
-      </c>
-      <c r="AE2" s="36" t="s">
-        <v>501</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="D3" s="85" t="s">
-        <v>850</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="F3" s="51" t="s">
-        <v>745</v>
-      </c>
-      <c r="G3" s="51" t="s">
-        <v>746</v>
-      </c>
-      <c r="H3" s="51" t="s">
-        <v>616</v>
-      </c>
-      <c r="I3" s="85" t="s">
-        <v>606</v>
-      </c>
-      <c r="J3" s="51" t="s">
-        <v>747</v>
-      </c>
-      <c r="K3" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="51" t="s">
-        <v>670</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>748</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>749</v>
-      </c>
-      <c r="P3" s="51" t="s">
-        <v>750</v>
-      </c>
-      <c r="Q3" s="51" t="s">
-        <v>751</v>
-      </c>
-      <c r="R3" s="23" t="s">
-        <v>752</v>
-      </c>
-      <c r="S3" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="X3" s="23" t="s">
-        <v>755</v>
-      </c>
-      <c r="Y3" s="23" t="s">
-        <v>609</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>756</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB3" s="23" t="s">
-        <v>757</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="AD3" s="36" t="s">
-        <v>500</v>
-      </c>
-      <c r="AE3" s="36" t="s">
-        <v>501</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5405,8 +5416,8 @@
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5419,7 +5430,7 @@
     <col min="6" max="6" width="25.109375" style="23" customWidth="1"/>
     <col min="7" max="7" width="11" style="23" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" style="23" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="35.21875" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="19.109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="29.44140625" style="3" customWidth="1"/>
     <col min="13" max="13" width="29.33203125" style="3" customWidth="1"/>
@@ -5459,106 +5470,106 @@
         <v>286</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="F1" s="54" t="s">
         <v>288</v>
       </c>
       <c r="G1" s="54" t="s">
+        <v>572</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>765</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>659</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>660</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>576</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>577</v>
+      </c>
+      <c r="N1" s="45" t="s">
         <v>578</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>586</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>763</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>656</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>657</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>582</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>583</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>584</v>
-      </c>
       <c r="O1" s="45" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="P1" s="28" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="S1" s="54" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="T1" s="54" t="s">
         <v>78</v>
       </c>
       <c r="U1" s="28" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="V1" s="28" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="W1" s="45" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="X1" s="45" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="Y1" s="45" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="AA1" s="26" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="AB1" s="26" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="AC1" s="26" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="AD1" s="46" t="s">
         <v>291</v>
       </c>
       <c r="AE1" s="46" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="AF1" s="46" t="s">
         <v>198</v>
       </c>
       <c r="AG1" s="46" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="AH1" s="45" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="AI1" s="45" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="AJ1" s="45" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="AK1" s="45" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5575,31 +5586,31 @@
         <v>469</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>775</v>
+      <c r="G2" s="85" t="s">
+        <v>852</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="I2" s="23" t="s">
-        <v>776</v>
+      <c r="I2" s="76" t="s">
+        <v>378</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>758</v>
+        <v>500</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>759</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>603</v>
+        <v>501</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>225</v>
@@ -5615,10 +5626,10 @@
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="23" t="s">
-        <v>777</v>
-      </c>
-      <c r="T2" s="23" t="s">
-        <v>778</v>
+        <v>779</v>
+      </c>
+      <c r="T2" s="76" t="s">
+        <v>851</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>550</v>
@@ -5630,46 +5641,46 @@
         <v>228</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="Z2" s="23" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="AA2" s="23" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="AB2" s="23" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="AC2" s="55" t="s">
-        <v>782</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>776</v>
+        <v>783</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AE2" s="36" t="s">
+        <v>500</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>377</v>
+      <c r="AG2" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="AH2" s="23" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
   </sheetData>
@@ -5686,8 +5697,8 @@
   </sheetPr>
   <dimension ref="A1:BI5"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5698,7 +5709,7 @@
     <col min="4" max="4" width="31.6640625" style="57" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="57" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" style="57" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="57" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="57" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="57" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" style="57" customWidth="1"/>
     <col min="10" max="10" width="23.88671875" style="57" customWidth="1"/>
@@ -5737,82 +5748,82 @@
         <v>288</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="I1" s="56" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="L1" s="56" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="M1" s="56" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="N1" s="59" t="s">
         <v>291</v>
       </c>
       <c r="O1" s="56" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="P1" s="58" t="s">
         <v>298</v>
       </c>
       <c r="Q1" s="56" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="R1" s="56" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="S1" s="30" t="s">
         <v>527</v>
       </c>
       <c r="T1" s="58" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="U1" s="45" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="V1" s="45" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="W1" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="X1" s="22" t="s">
+        <v>577</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="Z1" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="AA1" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB1" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="AC1" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="Y1" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="Z1" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="AA1" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="AB1" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="AC1" s="22" t="s">
-        <v>589</v>
-      </c>
       <c r="AD1" s="56" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:61" s="36" customFormat="1" x14ac:dyDescent="0.3">
@@ -5832,23 +5843,23 @@
         <v>469</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>744</v>
+        <v>595</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="J2" s="52" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="K2" s="52"/>
       <c r="L2" s="57" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M2" s="60" t="s">
         <v>390</v>
@@ -5866,10 +5877,10 @@
         <v>228</v>
       </c>
       <c r="R2" s="61" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="S2" s="57" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>212</v>
@@ -5896,13 +5907,13 @@
         <v>33.68</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
@@ -5953,23 +5964,23 @@
         <v>469</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="J3" s="52" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="K3" s="52"/>
       <c r="L3" s="57" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M3" s="60" t="s">
         <v>390</v>
@@ -5987,10 +5998,10 @@
         <v>228</v>
       </c>
       <c r="R3" s="61" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="S3" s="57" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>212</v>
@@ -6017,13 +6028,13 @@
         <v>33.68</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
@@ -6074,23 +6085,23 @@
         <v>469</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>798</v>
+        <v>761</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="I4" s="52" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="J4" s="52" t="s">
         <v>799</v>
       </c>
       <c r="K4" s="52"/>
       <c r="L4" s="57" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M4" s="60" t="s">
         <v>390</v>
@@ -6111,7 +6122,7 @@
         <v>800</v>
       </c>
       <c r="S4" s="57" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>212</v>
@@ -6138,11 +6149,11 @@
         <v>94.8</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -6193,23 +6204,23 @@
         <v>469</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>801</v>
       </c>
       <c r="H5" s="52" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="I5" s="52" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="J5" s="52" t="s">
         <v>802</v>
       </c>
       <c r="K5" s="52"/>
       <c r="L5" s="57" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M5" s="60" t="s">
         <v>390</v>
@@ -6230,7 +6241,7 @@
         <v>803</v>
       </c>
       <c r="S5" s="57" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>212</v>
@@ -6254,14 +6265,14 @@
         <v>225</v>
       </c>
       <c r="AA5" s="39">
-        <v>88.133333333333326</v>
+        <v>94.8</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
@@ -6460,7 +6471,7 @@
         <v>286</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E1" s="62" t="s">
         <v>288</v>
@@ -6490,7 +6501,7 @@
         <v>811</v>
       </c>
       <c r="N1" s="62" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="O1" s="62" t="s">
         <v>812</v>
@@ -6499,7 +6510,7 @@
         <v>813</v>
       </c>
       <c r="Q1" s="62" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="R1" s="62" t="s">
         <v>814</v>
@@ -6508,37 +6519,37 @@
         <v>291</v>
       </c>
       <c r="T1" s="56" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="U1" s="58" t="s">
         <v>298</v>
       </c>
       <c r="V1" s="65" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="W1" s="65" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="X1" s="65" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="Y1" s="22" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="Z1" s="22" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="AA1" s="22" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="AC1" s="62" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="AD1" s="62" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="AE1" s="62" t="s">
         <v>815</v>
@@ -6580,13 +6591,13 @@
         <v>827</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="AS1" s="62" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="AT1" s="62" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
     </row>
     <row r="2" spans="1:221" x14ac:dyDescent="0.3">
@@ -6612,7 +6623,7 @@
         <v>830</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="I2" s="64" t="s">
         <v>831</v>
@@ -6621,7 +6632,7 @@
         <v>832</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="L2" s="64" t="s">
         <v>833</v>
@@ -6630,7 +6641,7 @@
         <v>834</v>
       </c>
       <c r="N2" s="63" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="O2" s="64" t="s">
         <v>835</v>
@@ -6657,16 +6668,16 @@
         <v>838</v>
       </c>
       <c r="W2" s="36" t="s">
-        <v>758</v>
+        <v>777</v>
       </c>
       <c r="X2" s="36" t="s">
-        <v>759</v>
+        <v>778</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>225</v>
@@ -6681,7 +6692,7 @@
         <v>839</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AF2" s="63" t="s">
         <v>840</v>
@@ -6699,31 +6710,31 @@
         <v>840</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="AQ2" s="63" t="s">
         <v>390</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="AS2" s="63" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="AT2" s="63" t="s">
         <v>841</v>
@@ -6944,13 +6955,13 @@
         <v>828</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="D3" s="63" t="s">
         <v>469</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="F3" s="66" t="s">
         <v>829</v>
@@ -6968,7 +6979,7 @@
         <v>832</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="L3" s="64" t="s">
         <v>833</v>
@@ -6977,7 +6988,7 @@
         <v>834</v>
       </c>
       <c r="N3" s="63" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="O3" s="64" t="s">
         <v>835</v>
@@ -7004,16 +7015,16 @@
         <v>838</v>
       </c>
       <c r="W3" s="36" t="s">
-        <v>758</v>
+        <v>777</v>
       </c>
       <c r="X3" s="36" t="s">
-        <v>759</v>
+        <v>778</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="AA3" s="3" t="s">
         <v>225</v>
@@ -7028,7 +7039,7 @@
         <v>839</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AF3" s="63" t="s">
         <v>840</v>
@@ -7046,31 +7057,31 @@
         <v>840</v>
       </c>
       <c r="AK3" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="AQ3" s="63" t="s">
         <v>390</v>
       </c>
       <c r="AR3" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="AS3" s="63" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="AT3" s="63" t="s">
         <v>841</v>
@@ -8219,8 +8230,8 @@
   </sheetPr>
   <dimension ref="A1:CI3"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8899,8 +8910,8 @@
   </sheetPr>
   <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO34" sqref="AO34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9362,8 +9373,8 @@
   </sheetPr>
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9667,14 +9678,270 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
+      <c r="C5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5" t="s">
+        <v>464</v>
+      </c>
+      <c r="E5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
+      <c r="C6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D6" t="s">
+        <v>464</v>
+      </c>
+      <c r="E6" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
+      <c r="C7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D7" t="s">
+        <v>464</v>
+      </c>
+      <c r="E7" t="s">
+        <v>373</v>
+      </c>
     </row>
-    <row r="28" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D8" t="s">
+        <v>464</v>
+      </c>
+      <c r="E8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>371</v>
+      </c>
+      <c r="D9" t="s">
+        <v>464</v>
+      </c>
+      <c r="E9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" t="s">
+        <v>464</v>
+      </c>
+      <c r="E10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>371</v>
+      </c>
+      <c r="D11" t="s">
+        <v>464</v>
+      </c>
+      <c r="E11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>371</v>
+      </c>
+      <c r="D12" t="s">
+        <v>464</v>
+      </c>
+      <c r="E12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>371</v>
+      </c>
+      <c r="D13" t="s">
+        <v>464</v>
+      </c>
+      <c r="E13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D14" t="s">
+        <v>464</v>
+      </c>
+      <c r="E14" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>371</v>
+      </c>
+      <c r="D15" t="s">
+        <v>464</v>
+      </c>
+      <c r="E15" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>371</v>
+      </c>
+      <c r="D16" t="s">
+        <v>464</v>
+      </c>
+      <c r="E16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>371</v>
+      </c>
+      <c r="D17" t="s">
+        <v>464</v>
+      </c>
+      <c r="E17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D18" t="s">
+        <v>464</v>
+      </c>
+      <c r="E18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>371</v>
+      </c>
+      <c r="D19" t="s">
+        <v>464</v>
+      </c>
+      <c r="E19" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" t="s">
+        <v>464</v>
+      </c>
+      <c r="E20" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" t="s">
+        <v>464</v>
+      </c>
+      <c r="E21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" t="s">
+        <v>464</v>
+      </c>
+      <c r="E22" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>371</v>
+      </c>
+      <c r="D23" t="s">
+        <v>464</v>
+      </c>
+      <c r="E23" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>371</v>
+      </c>
+      <c r="D24" t="s">
+        <v>464</v>
+      </c>
+      <c r="E24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>371</v>
+      </c>
+      <c r="D25" t="s">
+        <v>464</v>
+      </c>
+      <c r="E25" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>371</v>
+      </c>
+      <c r="D26" t="s">
+        <v>464</v>
+      </c>
+      <c r="E26" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>371</v>
+      </c>
+      <c r="D27" t="s">
+        <v>464</v>
+      </c>
+      <c r="E27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>371</v>
+      </c>
+      <c r="D28" t="s">
+        <v>464</v>
+      </c>
+      <c r="E28" t="s">
+        <v>373</v>
+      </c>
       <c r="M28" s="76"/>
     </row>
   </sheetData>
@@ -9691,7 +9958,7 @@
   </sheetPr>
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
@@ -10713,107 +10980,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.88671875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="26" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>572</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>573</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>574</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>575</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10860,76 +11030,76 @@
         <v>288</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>298</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>484</v>
       </c>
       <c r="J1" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>577</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="P1" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="R1" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="S1" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="T1" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="U1" s="6" t="s">
         <v>586</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="V1" s="6" t="s">
         <v>587</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="W1" s="6" t="s">
         <v>588</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="X1" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>590</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>591</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>592</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>593</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>594</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>595</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>596</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>597</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>598</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10937,7 +11107,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>371</v>
@@ -10946,7 +11116,7 @@
         <v>464</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>473</v>
@@ -10964,10 +11134,10 @@
         <v>501</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>225</v>
@@ -10982,10 +11152,10 @@
         <v>33.68</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>469</v>
@@ -10994,25 +11164,25 @@
         <v>228</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="V2" s="76" t="s">
-        <v>384</v>
+        <v>601</v>
       </c>
       <c r="W2" s="76" t="s">
         <v>468</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11020,7 +11190,7 @@
         <v>417</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>371</v>
@@ -11029,7 +11199,7 @@
         <v>464</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>473</v>
@@ -11047,10 +11217,10 @@
         <v>501</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>225</v>
@@ -11065,10 +11235,10 @@
         <v>33.68</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>469</v>
@@ -11077,25 +11247,25 @@
         <v>228</v>
       </c>
       <c r="U3" s="29" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="V3" s="76" t="s">
-        <v>384</v>
+        <v>601</v>
       </c>
       <c r="W3" s="76" t="s">
         <v>468</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11103,7 +11273,7 @@
         <v>511</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>371</v>
@@ -11112,7 +11282,7 @@
         <v>373</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>473</v>
@@ -11130,10 +11300,10 @@
         <v>501</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>225</v>
@@ -11148,7 +11318,7 @@
         <v>94.8</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>469</v>
@@ -11157,25 +11327,25 @@
         <v>228</v>
       </c>
       <c r="U4" s="29" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="V4" s="76" t="s">
-        <v>384</v>
+        <v>612</v>
       </c>
       <c r="W4" s="76" t="s">
         <v>468</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11183,7 +11353,7 @@
         <v>551</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>371</v>
@@ -11192,7 +11362,7 @@
         <v>373</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>473</v>
@@ -11210,10 +11380,10 @@
         <v>501</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>225</v>
@@ -11225,10 +11395,10 @@
         <v>390</v>
       </c>
       <c r="P5" s="39">
-        <v>88.133333333333326</v>
+        <v>94.8</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>469</v>
@@ -11237,19 +11407,19 @@
         <v>228</v>
       </c>
       <c r="U5" s="29" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="V5" s="76" t="s">
-        <v>384</v>
+        <v>617</v>
       </c>
       <c r="W5" s="76" t="s">
         <v>468</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>555</v>
@@ -11258,7 +11428,7 @@
         <v>165</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -11272,6 +11442,103 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E12" s="44"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="26" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>619</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>622</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -11345,34 +11612,34 @@
         <v>354</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>357</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="O1" s="34" t="s">
         <v>359</v>
@@ -11387,31 +11654,31 @@
         <v>362</v>
       </c>
       <c r="S1" s="34" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="T1" s="34" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="U1" s="34" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="W1" s="34" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="X1" s="38" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="Y1" s="38" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="Z1" s="38" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="AA1" s="38" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="AB1" s="38"/>
       <c r="AC1" s="38"/>
@@ -11431,63 +11698,63 @@
         <v>499</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>406</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>228</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>410</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="K2" s="39"/>
       <c r="L2" s="7" t="s">
         <v>554</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="29" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>209</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="R2" s="7">
         <v>100</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>222</v>
@@ -11496,13 +11763,13 @@
         <v>481</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>281</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>